<commit_message>
subgenomic RNA in bulk phase was added
</commit_message>
<xml_diff>
--- a/src/Cov19_life_cycle/cov19_life_cycle.xlsx
+++ b/src/Cov19_life_cycle/cov19_life_cycle.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39116EBB-534A-4AF6-8EC2-E58A0AEDF8E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6993B8-A462-4FA2-AE17-98298E421F4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Reaction" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Reaction!$A$4:$K$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Reaction!$A$4:$K$43</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="411">
   <si>
     <t>on</t>
   </si>
@@ -449,9 +449,6 @@
     <t>entry of COV into iPC with concomitant ACE2 degradation</t>
   </si>
   <si>
-    <t>degradation of COV_ACE2 located at PC with concomitant COV release to bulk phase via PC apoptosis</t>
-  </si>
-  <si>
     <t>COV_ACE2_ipc = COV_ipc</t>
   </si>
   <si>
@@ -482,12 +479,6 @@
     <t>degradation of ACE2 located at iPC via iPC apoptosis</t>
   </si>
   <si>
-    <t>degradation of COV_ACE2 located at iPC with concomitant COV release to bulk phase via iPC apoptosis</t>
-  </si>
-  <si>
-    <t>degradation of COV located in iPC with concomitant COV release to bulk phase via iPC apoptosis</t>
-  </si>
-  <si>
     <t>V_ent_cov_ipc</t>
   </si>
   <si>
@@ -518,9 +509,6 @@
     <t>V_deg_cov_apo_vpc</t>
   </si>
   <si>
-    <t>degradation of COV located in vPC with concomitant COV release to bulk phase via vPC apoptosis</t>
-  </si>
-  <si>
     <t>V_deg_cov_rna_apo_vpc</t>
   </si>
   <si>
@@ -1007,9 +995,6 @@
     <t>k_apo_pc*COV_ACE2_vpc</t>
   </si>
   <si>
-    <t>degradation of COV_ACE2 located at vPC with concomitant COV release to bulk phase via vPC apoptosis</t>
-  </si>
-  <si>
     <t>k_ent_cov_ipc*COV_ACE2_vpc</t>
   </si>
   <si>
@@ -1221,6 +1206,63 @@
   </si>
   <si>
     <t xml:space="preserve">maximal number of virions Nmax = (surface area of PC faced to alveoli lumen)/(area of "maximal" section of SARS-CoV-2). Based on PC surface area = 183 um^2 [7103258] and (virion diameter=120-160 nm), one obtains Nmax =  183 um^2 / Pi*(140/2 nm) ^2 = 11900 </t>
+  </si>
+  <si>
+    <t>COV_RNA_vpc=COV_RNA</t>
+  </si>
+  <si>
+    <t>degradation of COV_RNA located at vPC with concomitant COV_RNA release to bulk phase via vPC apoptosis</t>
+  </si>
+  <si>
+    <t>V_deg_cov_rna</t>
+  </si>
+  <si>
+    <t>COV_RNA=</t>
+  </si>
+  <si>
+    <t>degradation of COV_RNA in bulk phase</t>
+  </si>
+  <si>
+    <t>degradation of COV_ACE2 located at PC via PC apoptosis</t>
+  </si>
+  <si>
+    <t>degradation of COV_ACE2 located at iPC via iPC apoptosis</t>
+  </si>
+  <si>
+    <t>degradation of COV located in iPC via iPC apoptosis</t>
+  </si>
+  <si>
+    <t>degradation of COV_ACE2 located at vPC via vPC apoptosis</t>
+  </si>
+  <si>
+    <t>degradation of COV located in vPC via vPC apoptosis</t>
+  </si>
+  <si>
+    <t>COV_RNA</t>
+  </si>
+  <si>
+    <t>concentration of COV_RNA released from vPC due to their apoptosis</t>
+  </si>
+  <si>
+    <t>Vol_alv*k_deg_cov_rna*COV_RNA</t>
+  </si>
+  <si>
+    <t>k_deg_cov_rna</t>
+  </si>
+  <si>
+    <t>rate constant of COV_RNA degradation in bulk phase</t>
+  </si>
+  <si>
+    <t>assumed to be equal to COV half-life equal to 4 hour. So, rate constant is equal to ln2/4 = 0.17 1/h</t>
+  </si>
+  <si>
+    <t>COV_sgRNA_perc</t>
+  </si>
+  <si>
+    <t>100*COV_RNA/COV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent of actively transcribed subgenomic RNA of total (packed + unpacked) RNA in sputum samples taken from the patients </t>
   </si>
 </sst>
 </file>
@@ -1673,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1778,13 +1820,13 @@
         <v>1000</v>
       </c>
       <c r="F5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="J5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="K5" t="s">
         <v>43</v>
@@ -1798,19 +1840,19 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E6" s="6">
         <v>602000000000</v>
       </c>
       <c r="F6" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="H6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="K6" t="s">
         <v>43</v>
@@ -1836,7 +1878,7 @@
         <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="J7" t="s">
         <v>65</v>
@@ -1845,7 +1887,7 @@
         <v>90</v>
       </c>
       <c r="L7" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1868,7 +1910,7 @@
         <v>103</v>
       </c>
       <c r="I8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J8" t="s">
         <v>65</v>
@@ -1877,7 +1919,7 @@
         <v>90</v>
       </c>
       <c r="L8" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1888,19 +1930,19 @@
         <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E9" s="5">
         <v>0.01</v>
       </c>
       <c r="F9" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H9" t="s">
         <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="J9" t="s">
         <v>65</v>
@@ -1917,19 +1959,19 @@
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E10" s="5">
         <v>0.01</v>
       </c>
       <c r="F10" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H10" t="s">
         <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="J10" t="s">
         <v>65</v>
@@ -1946,7 +1988,7 @@
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E11" s="10">
         <v>1.8</v>
@@ -1955,10 +1997,10 @@
         <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="I11" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="J11" t="s">
         <v>116</v>
@@ -1970,7 +2012,7 @@
         <v>20463877</v>
       </c>
       <c r="M11" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1981,7 +2023,7 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E12" s="6">
         <v>23.56</v>
@@ -1990,10 +2032,10 @@
         <v>67</v>
       </c>
       <c r="H12" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I12" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="J12" t="s">
         <v>116</v>
@@ -2005,7 +2047,7 @@
         <v>32225176</v>
       </c>
       <c r="M12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -2016,19 +2058,19 @@
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E13" s="6">
         <v>31.13</v>
       </c>
       <c r="F13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H13" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I13" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="J13" t="s">
         <v>116</v>
@@ -2040,7 +2082,7 @@
         <v>32225176</v>
       </c>
       <c r="M13" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -2051,7 +2093,7 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E14" s="8">
         <v>0.93600000000000005</v>
@@ -2060,13 +2102,13 @@
         <v>67</v>
       </c>
       <c r="H14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I14" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="J14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K14" t="s">
         <v>90</v>
@@ -2075,7 +2117,7 @@
         <v>9894006</v>
       </c>
       <c r="M14" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -2087,7 +2129,7 @@
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E15" s="8">
         <v>1</v>
@@ -2097,13 +2139,13 @@
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K15" s="11" t="s">
         <v>43</v>
@@ -2112,7 +2154,7 @@
         <v>15384040</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -2123,7 +2165,7 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E16" s="8">
         <v>0.6</v>
@@ -2132,22 +2174,22 @@
         <v>67</v>
       </c>
       <c r="H16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I16" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="J16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K16" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="L16" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="M16" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -2158,7 +2200,7 @@
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E17" s="8">
         <v>14</v>
@@ -2167,13 +2209,13 @@
         <v>67</v>
       </c>
       <c r="H17" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="J17" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K17" t="s">
         <v>43</v>
@@ -2182,7 +2224,7 @@
         <v>15384040</v>
       </c>
       <c r="M17" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -2194,7 +2236,7 @@
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E18" s="10">
         <v>3.7999999999999999E-2</v>
@@ -2204,22 +2246,22 @@
       </c>
       <c r="G18" s="11"/>
       <c r="H18" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="L18" s="11">
         <v>15384040</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -2230,7 +2272,7 @@
         <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E19" s="10">
         <v>0.6</v>
@@ -2239,22 +2281,22 @@
         <v>67</v>
       </c>
       <c r="H19" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I19" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="J19" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K19" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="L19" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="M19" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2265,31 +2307,31 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E20" s="10">
         <v>10000</v>
       </c>
       <c r="F20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H20" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I20" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="J20" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K20" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="L20">
         <v>15384040</v>
       </c>
       <c r="M20" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2301,7 +2343,7 @@
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E21" s="10">
         <v>0.14000000000000001</v>
@@ -2311,22 +2353,22 @@
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="L21" s="11">
         <v>15384040</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -2337,7 +2379,7 @@
         <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E22" s="10">
         <v>1</v>
@@ -2346,22 +2388,22 @@
         <v>67</v>
       </c>
       <c r="H22" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I22" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="J22" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K22" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="L22" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="M22" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2372,7 +2414,7 @@
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E23" s="6">
         <v>0.17</v>
@@ -2381,13 +2423,13 @@
         <v>67</v>
       </c>
       <c r="H23" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I23" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="J23" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K23" t="s">
         <v>90</v>
@@ -2396,7 +2438,7 @@
         <v>32182409</v>
       </c>
       <c r="M23" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -2407,19 +2449,19 @@
         <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E24" s="6">
         <v>11900</v>
       </c>
       <c r="F24" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H24" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I24" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="J24" t="s">
         <v>116</v>
@@ -2431,7 +2473,36 @@
         <v>7103258</v>
       </c>
       <c r="M24" t="s">
-        <v>223</v>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>405</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" t="s">
+        <v>406</v>
+      </c>
+      <c r="I25" t="s">
+        <v>407</v>
+      </c>
+      <c r="J25" t="s">
+        <v>161</v>
+      </c>
+      <c r="K25" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="8:8" x14ac:dyDescent="0.3">
@@ -2447,10 +2518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2542,23 +2613,23 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="I5" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="K5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2566,20 +2637,20 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K6" t="s">
         <v>116</v>
@@ -2590,19 +2661,19 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
         <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="G7" t="s">
         <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="K7" t="s">
         <v>116</v>
@@ -2613,19 +2684,19 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D8" t="s">
         <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="G8" t="s">
         <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="K8" t="s">
         <v>116</v>
@@ -2636,19 +2707,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F9" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="K9" t="s">
         <v>116</v>
@@ -2659,19 +2730,19 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D10" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F10" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G10" t="s">
+        <v>265</v>
+      </c>
+      <c r="I10" t="s">
         <v>269</v>
-      </c>
-      <c r="I10" t="s">
-        <v>273</v>
       </c>
       <c r="K10" t="s">
         <v>116</v>
@@ -2682,22 +2753,22 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D11" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G11" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I11" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="K11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2705,22 +2776,22 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D12" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="G12" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I12" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="K12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2728,22 +2799,22 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D13" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F13" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G13" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I13" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="K13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2751,22 +2822,22 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D14" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="F14" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G14" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I14" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="K14" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2774,22 +2845,22 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D15" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F15" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="G15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I15" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K15" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2797,22 +2868,22 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D16" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F16" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="G16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I16" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="K16" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -2820,22 +2891,22 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D17" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F17" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="G17" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I17" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="K17" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -2843,22 +2914,22 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D18" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F18" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G18" t="s">
+        <v>256</v>
+      </c>
+      <c r="I18" t="s">
         <v>260</v>
       </c>
-      <c r="I18" t="s">
-        <v>264</v>
-      </c>
       <c r="K18" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -2866,19 +2937,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D19" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F19" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G19" t="s">
         <v>40</v>
       </c>
       <c r="I19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="K19" t="s">
         <v>65</v>
@@ -2889,19 +2960,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D20" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F20" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G20" t="s">
         <v>89</v>
       </c>
       <c r="I20" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="K20" t="s">
         <v>65</v>
@@ -2912,19 +2983,19 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D21" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="F21" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="G21" t="s">
         <v>89</v>
       </c>
       <c r="I21" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="K21" t="s">
         <v>65</v>
@@ -2935,19 +3006,19 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D22" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="F22" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="G22" t="s">
         <v>89</v>
       </c>
       <c r="I22" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="K22" t="s">
         <v>65</v>
@@ -2958,22 +3029,22 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D23" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F23" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="G23" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I23" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="K23" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -2981,22 +3052,22 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D24" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="F24" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G24" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I24" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="K24" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -3004,22 +3075,22 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D25" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F25" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="G25" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I25" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="K25" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -3027,19 +3098,19 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D26" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F26" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="G26" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I26" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="K26" t="s">
         <v>75</v>
@@ -3050,19 +3121,19 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D27" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="F27" t="s">
+        <v>361</v>
+      </c>
+      <c r="G27" t="s">
+        <v>265</v>
+      </c>
+      <c r="I27" t="s">
         <v>366</v>
-      </c>
-      <c r="G27" t="s">
-        <v>269</v>
-      </c>
-      <c r="I27" t="s">
-        <v>371</v>
       </c>
       <c r="K27" t="s">
         <v>75</v>
@@ -3073,19 +3144,19 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D28" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="F28" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="G28" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I28" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="K28" t="s">
         <v>75</v>
@@ -3096,19 +3167,19 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D29" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F29" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="G29" t="s">
         <v>89</v>
       </c>
       <c r="I29" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="K29" t="s">
         <v>116</v>
@@ -3119,22 +3190,22 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D30" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="F30" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="G30" t="s">
         <v>89</v>
       </c>
       <c r="I30" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="K30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -3142,22 +3213,45 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D31" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F31" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G31" t="s">
         <v>89</v>
       </c>
       <c r="I31" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="K31" t="s">
-        <v>165</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>254</v>
+      </c>
+      <c r="D32" t="s">
+        <v>408</v>
+      </c>
+      <c r="F32" t="s">
+        <v>409</v>
+      </c>
+      <c r="G32" t="s">
+        <v>89</v>
+      </c>
+      <c r="I32" t="s">
+        <v>410</v>
+      </c>
+      <c r="K32" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3307,19 +3401,19 @@
         <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J6" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="L6" t="s">
         <v>90</v>
       </c>
       <c r="M6" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="N6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -3330,7 +3424,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E7" s="7">
         <v>0.26700000000000002</v>
@@ -3342,10 +3436,10 @@
         <v>87</v>
       </c>
       <c r="J7" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M7" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -3362,13 +3456,13 @@
         <v>1.33E-12</v>
       </c>
       <c r="G8" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I8" t="s">
         <v>85</v>
       </c>
       <c r="J8" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="L8" t="s">
         <v>90</v>
@@ -3377,7 +3471,7 @@
         <v>7103258</v>
       </c>
       <c r="N8" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3387,10 +3481,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3524,10 +3618,10 @@
         <v>78</v>
       </c>
       <c r="K5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="L5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="M5" t="s">
         <v>65</v>
@@ -3539,7 +3633,7 @@
         <v>7103258</v>
       </c>
       <c r="P5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -3562,7 +3656,7 @@
         <v>78</v>
       </c>
       <c r="K6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="M6" t="s">
         <v>65</v>
@@ -3588,7 +3682,7 @@
         <v>78</v>
       </c>
       <c r="K7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="M7" t="s">
         <v>65</v>
@@ -3617,10 +3711,10 @@
         <v>78</v>
       </c>
       <c r="K8" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="L8" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="M8" t="s">
         <v>65</v>
@@ -3632,7 +3726,7 @@
         <v>7103258</v>
       </c>
       <c r="P8" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -3643,13 +3737,13 @@
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E9" s="9">
         <v>615</v>
       </c>
       <c r="G9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I9" t="s">
         <v>78</v>
@@ -3658,10 +3752,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="L9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="M9" t="s">
         <v>116</v>
@@ -3678,13 +3772,13 @@
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E10" s="9">
         <v>615</v>
       </c>
       <c r="G10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>
@@ -3696,10 +3790,10 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="L10" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="M10" t="s">
         <v>116</v>
@@ -3716,13 +3810,13 @@
         <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I11" t="s">
         <v>78</v>
@@ -3731,7 +3825,7 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="M11" t="s">
         <v>116</v>
@@ -3745,13 +3839,13 @@
         <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I12" t="s">
         <v>78</v>
@@ -3760,10 +3854,10 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="M12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -3774,13 +3868,13 @@
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I13" t="s">
         <v>78</v>
@@ -3789,10 +3883,10 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -3803,13 +3897,13 @@
         <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I14" t="s">
         <v>78</v>
@@ -3818,10 +3912,10 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -3832,13 +3926,13 @@
         <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I15" t="s">
         <v>78</v>
@@ -3847,10 +3941,10 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="M15" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -3861,13 +3955,13 @@
         <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I16" t="s">
         <v>78</v>
@@ -3876,10 +3970,10 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="M16" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -3890,13 +3984,13 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I17" t="s">
         <v>78</v>
@@ -3905,10 +3999,10 @@
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M17" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -3919,13 +4013,13 @@
         <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I18" t="s">
         <v>78</v>
@@ -3934,10 +4028,10 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="M18" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -3954,16 +4048,42 @@
         <v>2E-3</v>
       </c>
       <c r="G19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I19" t="s">
         <v>78</v>
       </c>
       <c r="K19" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="M19" t="s">
-        <v>165</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>402</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>145</v>
+      </c>
+      <c r="I20" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" t="s">
+        <v>403</v>
+      </c>
+      <c r="M20" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3974,10 +4094,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4102,7 +4222,7 @@
         <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F6" t="s">
         <v>53</v>
@@ -4128,7 +4248,7 @@
         <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F7" t="s">
         <v>53</v>
@@ -4255,10 +4375,10 @@
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F12" t="s">
         <v>92</v>
@@ -4267,7 +4387,7 @@
         <v>94</v>
       </c>
       <c r="I12" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="K12" t="s">
         <v>116</v>
@@ -4284,7 +4404,7 @@
         <v>97</v>
       </c>
       <c r="E13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F13" t="s">
         <v>92</v>
@@ -4342,10 +4462,10 @@
         <v>92</v>
       </c>
       <c r="G15" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I15" t="s">
-        <v>139</v>
+        <v>397</v>
       </c>
       <c r="K15" t="s">
         <v>116</v>
@@ -4414,7 +4534,7 @@
         <v>117</v>
       </c>
       <c r="E18" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F18" t="s">
         <v>92</v>
@@ -4423,10 +4543,10 @@
         <v>127</v>
       </c>
       <c r="I18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -4437,10 +4557,10 @@
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E19" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F19" t="s">
         <v>92</v>
@@ -4449,10 +4569,10 @@
         <v>128</v>
       </c>
       <c r="I19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="K19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -4466,7 +4586,7 @@
         <v>118</v>
       </c>
       <c r="E20" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F20" t="s">
         <v>92</v>
@@ -4475,10 +4595,10 @@
         <v>129</v>
       </c>
       <c r="I20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -4501,10 +4621,10 @@
         <v>128</v>
       </c>
       <c r="I21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -4524,13 +4644,13 @@
         <v>92</v>
       </c>
       <c r="G22" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="I22" t="s">
-        <v>150</v>
+        <v>398</v>
       </c>
       <c r="K22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -4550,13 +4670,13 @@
         <v>92</v>
       </c>
       <c r="G23" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="I23" t="s">
-        <v>151</v>
+        <v>399</v>
       </c>
       <c r="K23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -4567,7 +4687,7 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E24" t="s">
         <v>137</v>
@@ -4576,13 +4696,13 @@
         <v>92</v>
       </c>
       <c r="G24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I24" t="s">
         <v>138</v>
       </c>
       <c r="K24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -4594,24 +4714,24 @@
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="12" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -4636,11 +4756,11 @@
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -4655,7 +4775,7 @@
         <v>126</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>92</v>
@@ -4665,11 +4785,11 @@
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -4681,24 +4801,24 @@
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>141</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>142</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -4719,15 +4839,15 @@
         <v>92</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -4739,24 +4859,24 @@
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>313</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>317</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -4771,21 +4891,21 @@
         <v>122</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -4800,21 +4920,21 @@
         <v>123</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -4829,21 +4949,21 @@
         <v>124</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="12" t="s">
-        <v>325</v>
+        <v>400</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -4855,24 +4975,24 @@
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="12" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -4884,24 +5004,24 @@
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J35" s="12"/>
       <c r="K35" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -4912,22 +5032,22 @@
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E36" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F36" t="s">
         <v>92</v>
       </c>
       <c r="G36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K36" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -4938,22 +5058,22 @@
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E37" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F37" t="s">
         <v>92</v>
       </c>
       <c r="G37" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I37" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="K37" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -4964,22 +5084,22 @@
         <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E38" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F38" t="s">
         <v>92</v>
       </c>
       <c r="G38" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I38" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K38" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -4990,48 +5110,51 @@
         <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E39" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F39" t="s">
         <v>92</v>
       </c>
       <c r="G39" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I39" t="s">
-        <v>162</v>
+        <v>401</v>
       </c>
       <c r="K39" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="A40" s="11">
+        <v>0</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C40" s="11"/>
+      <c r="D40" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E40" t="s">
-        <v>167</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="F40" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G40" t="s">
-        <v>388</v>
-      </c>
-      <c r="I40" t="s">
-        <v>164</v>
-      </c>
-      <c r="K40" t="s">
-        <v>165</v>
+      <c r="G40" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -5042,26 +5165,78 @@
         <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>52</v>
+        <v>159</v>
       </c>
       <c r="E41" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="F41" t="s">
         <v>92</v>
       </c>
       <c r="G41" t="s">
-        <v>169</v>
+        <v>392</v>
       </c>
       <c r="I41" t="s">
-        <v>170</v>
+        <v>393</v>
       </c>
       <c r="K41" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" t="s">
         <v>165</v>
       </c>
+      <c r="I42" t="s">
+        <v>166</v>
+      </c>
+      <c r="K42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" t="s">
+        <v>394</v>
+      </c>
+      <c r="E43" t="s">
+        <v>404</v>
+      </c>
+      <c r="F43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" t="s">
+        <v>395</v>
+      </c>
+      <c r="I43" t="s">
+        <v>396</v>
+      </c>
+      <c r="K43" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:K41" xr:uid="{6674B1C7-2B72-4099-8A9D-5016CD5D9EBF}"/>
+  <autoFilter ref="A4:K43" xr:uid="{6674B1C7-2B72-4099-8A9D-5016CD5D9EBF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
version 0.1.2 was developed
</commit_message>
<xml_diff>
--- a/src/Cov19_life_cycle/cov19_life_cycle.xlsx
+++ b/src/Cov19_life_cycle/cov19_life_cycle.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6993B8-A462-4FA2-AE17-98298E421F4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE9DC7E-A6B3-4DF8-8999-CB99EC76F7C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Reaction" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Reaction!$A$4:$K$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Reaction!$A$4:$K$49</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="475">
   <si>
     <t>on</t>
   </si>
@@ -602,12 +602,6 @@
     <t>COV_vpc</t>
   </si>
   <si>
-    <t>amount of COV particles located in iPC</t>
-  </si>
-  <si>
-    <t>amount of COV particles located in vPC</t>
-  </si>
-  <si>
     <t>k_ent_cov_ipc</t>
   </si>
   <si>
@@ -659,15 +653,9 @@
     <t xml:space="preserve">release of COV in iPC </t>
   </si>
   <si>
-    <t>k_rel_cov_ipc</t>
-  </si>
-  <si>
     <t>rate constant of COV release to bulk phase from iPC and vPC cell</t>
   </si>
   <si>
-    <t>k_rel_cov_ipc*COV_ipc</t>
-  </si>
-  <si>
     <t>k_rel_cov_ipc*COV_vpc</t>
   </si>
   <si>
@@ -716,9 +704,6 @@
     <t>k_off for viral Spike receptor binding domain (RBD) and ACE2 receptor</t>
   </si>
   <si>
-    <t>Kd for viral Spike receptor binding domain (RBD) and ACE2 receptor is equal to 4.67 nM. Basing on estimate that virion includes about 150 spike proteins (virion diameter=120-160 nm, Spike height=20nm) we have calculated Kd for COV and ACE2 binding equal to 4.67 nM/150 = 31.13 pM</t>
-  </si>
-  <si>
     <t>Fig 1</t>
   </si>
   <si>
@@ -752,9 +737,6 @@
     <t xml:space="preserve">characteristic time of "virus assembly/budding" was estimated as 1 h for Influenza virus. Since Influenza and SARS-CoV-2 have different "incubation period" (2-3 days vs 14 days) we have estimated SARS-CoV-2 "replication" characteristic time as 5 h. </t>
   </si>
   <si>
-    <t xml:space="preserve">it was proposed that a host cell can produce about 8000 virions of Influenza virus before it dies. So we have calculated the EC50 basing on the value.  </t>
-  </si>
-  <si>
     <t>table 3</t>
   </si>
   <si>
@@ -986,15 +968,9 @@
     <t>binding of COV to ACE2 located at vPC surface</t>
   </si>
   <si>
-    <t>k_apo_pc*ACE2_vpc</t>
-  </si>
-  <si>
     <t>degradation of ACE2 located at iPC via vPC apoptosis</t>
   </si>
   <si>
-    <t>k_apo_pc*COV_ACE2_vpc</t>
-  </si>
-  <si>
     <t>k_ent_cov_ipc*COV_ACE2_vpc</t>
   </si>
   <si>
@@ -1259,10 +1235,226 @@
     <t>COV_sgRNA_perc</t>
   </si>
   <si>
-    <t>100*COV_RNA/COV</t>
-  </si>
-  <si>
     <t xml:space="preserve">percent of actively transcribed subgenomic RNA of total (packed + unpacked) RNA in sputum samples taken from the patients </t>
+  </si>
+  <si>
+    <t>COVass_vpc</t>
+  </si>
+  <si>
+    <t>amount of assembled virus ready to be released from from vPC</t>
+  </si>
+  <si>
+    <t>amount of partially disrupted COV particles ready to release RNA in cytoplasm located in vPC</t>
+  </si>
+  <si>
+    <t>amount of partially disrupted COV particles ready to release RNA in cytoplasm located in iPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COV_RNA_vpc = COVass_vpc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COVass_vpc = COV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it was proposed that a host cell can produce about 8000 (item/cell) virions of Influenza virus before it dies [15384040]. So we have calculated the EC50 basing on the value; taking into account that Vol_pc = 1.33e-12 L/cell we can obtain estimate in pM: EC50 = 8e3 /NA_pmole/Vol_pc = 8e3/6.02e11/1.33e-12 = 9992 pM  </t>
+  </si>
+  <si>
+    <t>V_deg_cov_ass_apo_vpc</t>
+  </si>
+  <si>
+    <t>k_apo_vpc*COVass_vpc</t>
+  </si>
+  <si>
+    <t>degradation of COVass located in vPC via vPC apoptosis with concomitant COV release</t>
+  </si>
+  <si>
+    <t>COVass_vpc = COV</t>
+  </si>
+  <si>
+    <t>k_rel_cov_vpc*COVass_vpc</t>
+  </si>
+  <si>
+    <t>k_rel_cov_vpc</t>
+  </si>
+  <si>
+    <t>k_rel_cov_vpc*COV_ipc</t>
+  </si>
+  <si>
+    <t>k_apo_vpc*ACE2_vpc</t>
+  </si>
+  <si>
+    <t>k_apo_vpc*COV_ACE2_vpc</t>
+  </si>
+  <si>
+    <t>COV_ACE2_pc = COV</t>
+  </si>
+  <si>
+    <t>degradation of COV_ACE2 located at PC via PC apoptosis with concomitant COV release</t>
+  </si>
+  <si>
+    <t>COV_ACE2_ipc = COV</t>
+  </si>
+  <si>
+    <t>degradation of COV_ACE2 located at iPC via iPC apoptosis with concomitant COV release</t>
+  </si>
+  <si>
+    <t>COV_ACE2_vpc = COV</t>
+  </si>
+  <si>
+    <t>degradation of COV_ACE2 located at vPC via vPC apoptosis with concomitant COV release</t>
+  </si>
+  <si>
+    <t>100*COV_RNA/(COV + COV_RNA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100*COV_RNA/COV </t>
+  </si>
+  <si>
+    <t>COVass_vpc_per_cell</t>
+  </si>
+  <si>
+    <t>NA_pmole*COVass_vpc/vPC/Vol_alv/kcell_to_cell</t>
+  </si>
+  <si>
+    <t>number of COVass per vPC cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR_apo </t>
+  </si>
+  <si>
+    <t>empiric function imitating effect of Immune Response on vPC apoptosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kbase_apo_vpc*IR_apo</t>
+  </si>
+  <si>
+    <t>dependence of rate constant of vPC apoptosis on IR effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch_ir </t>
+  </si>
+  <si>
+    <t>T_sw_ir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emax_ir_apo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_ir </t>
+  </si>
+  <si>
+    <t>switch of effect of IR on vPC apoptosis</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>switch on time of IR effect on vPC apoptosis</t>
+  </si>
+  <si>
+    <t>ET50_ir</t>
+  </si>
+  <si>
+    <t>Effective Time when IR effect reach 50% of maximal value</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>maximal effect of IR on vPC apoptosis</t>
+  </si>
+  <si>
+    <t>Hill coefficient of IR effect on vPC apoptosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 + switch_ir*Emax_ir_apo*(t - T_sw_ir)^n_ir/((T_sw_ir + ET50_ir)^n_ir + (t - T_sw_ir)^n_ir)</t>
+  </si>
+  <si>
+    <t>kbase_apo_vpc</t>
+  </si>
+  <si>
+    <t>apparent dissociation equilibrium constant of COV and ACE2</t>
+  </si>
+  <si>
+    <t>VO</t>
+  </si>
+  <si>
+    <t>anti_Ab/(Kd_anti_Ab + anti_Ab)</t>
+  </si>
+  <si>
+    <t>Virus Occupancy (VO) level with anti_Ab antibodies</t>
+  </si>
+  <si>
+    <t>Kd for viral Spike receptor binding domain (RBD) and ACE2 receptor is known and equal to 4.67 nM. Basing on estimate that virion includes  VO*Num_sp_per_cov free spike proteins ready to bind to ACE2 we have come to the equation for apparent Kd describing binding of virion and ACE2</t>
+  </si>
+  <si>
+    <t>Kd_anti_Ab</t>
+  </si>
+  <si>
+    <t>anti_Ab</t>
+  </si>
+  <si>
+    <t>Kd_spike_ace2/Num_sp_per_cov/(1 - VO)</t>
+  </si>
+  <si>
+    <t>Kd_spike_ace2</t>
+  </si>
+  <si>
+    <t>equilibrium dissociation constant of spike (RBD) to ACE2 binding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kd for viral Spike receptor binding domain (RBD) and ACE2 </t>
+  </si>
+  <si>
+    <t>Num_sp_per_cov</t>
+  </si>
+  <si>
+    <t>number of Spike proteins per virion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basing on estimate  that virion diameter=120-160 nm and Spike height=20nm we have come to following number of Spikes per virion = 4*3.14*(70 nm)^2/(3.14*(10 nm)^2)  = 4*49 = 196. Assuming that "dynamic" diameter of Spike is little bit more we have assumed that there are about  150 spike proteins per 1 virion. </t>
+  </si>
+  <si>
+    <t>Kd for binding of Spike protein and neutralizing antibodies</t>
+  </si>
+  <si>
+    <t>assumed to be equal to tat presented in the paper for neutralizing mAb</t>
+  </si>
+  <si>
+    <t>concentration of anti-Spike attibodies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> switch_ir*anti_Ab_max*(t - T_sw_ir)^n_ir/((T_sw_ir + ET50_ir)^n_ir + (t - T_sw_ir)^n_ir)</t>
+  </si>
+  <si>
+    <t>hill like expression describes general kinetic pattern observed for Spike specific IgG and IgM in [32350462]</t>
+  </si>
+  <si>
+    <t>anti_Ab_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Protective Antigen (PA) for Anthrax vaccine it was measured that concentration of Anti-PA specific IgG in serum is 141.2 ug/mL [15358653]. Taking into account Mr_IgG = 150 kDa, one obtains 141.2 ug/mL =  </t>
+  </si>
+  <si>
+    <t>maximal concentration of anti Spike Ab in serum</t>
+  </si>
+  <si>
+    <t>number of virus copies in 1 mL of sputum</t>
+  </si>
+  <si>
+    <t>COV_num_sputum_ml</t>
+  </si>
+  <si>
+    <t>sputum_dilution_coef*(COV + COV_RNA)*Vol_alv*NA_pmole/1000</t>
+  </si>
+  <si>
+    <t>sputum_dilution_coef</t>
+  </si>
+  <si>
+    <t>dilution of sputum in comparison with lung epithelium lining fluid</t>
+  </si>
+  <si>
+    <t>SS???</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1494,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1339,6 +1531,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1361,7 +1559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1375,6 +1573,9 @@
     <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1713,10 +1914,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1820,7 +2024,7 @@
         <v>1000</v>
       </c>
       <c r="F5" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="H5" t="s">
         <v>182</v>
@@ -1840,16 +2044,16 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E6" s="6">
         <v>602000000000</v>
       </c>
       <c r="F6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="H6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="J6" t="s">
         <v>181</v>
@@ -1859,36 +2063,37 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
-        <v>64</v>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>472</v>
       </c>
       <c r="E7" s="6">
-        <v>8.1999999999999998E-4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I7" t="s">
-        <v>330</v>
-      </c>
-      <c r="J7" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" t="s">
-        <v>90</v>
-      </c>
-      <c r="L7" t="s">
-        <v>331</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1898,7 +2103,7 @@
         <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="E8" s="6">
         <v>8.1999999999999998E-4</v>
@@ -1907,10 +2112,10 @@
         <v>67</v>
       </c>
       <c r="H8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>222</v>
+        <v>322</v>
       </c>
       <c r="J8" t="s">
         <v>65</v>
@@ -1919,37 +2124,43 @@
         <v>90</v>
       </c>
       <c r="L8" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="11">
+        <v>0</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
-        <v>294</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="F9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" t="s">
-        <v>384</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="6">
+        <v>8.1999999999999998E-4</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="K9" t="s">
-        <v>42</v>
-      </c>
+      <c r="K9" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1959,61 +2170,62 @@
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>295</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.01</v>
+        <v>446</v>
+      </c>
+      <c r="E10" s="6">
+        <v>8.1999999999999998E-4</v>
       </c>
       <c r="F10" t="s">
-        <v>170</v>
+        <v>67</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="I10" t="s">
-        <v>384</v>
+        <v>218</v>
       </c>
       <c r="J10" t="s">
         <v>65</v>
       </c>
       <c r="K10" t="s">
+        <v>90</v>
+      </c>
+      <c r="L10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>0</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>242</v>
-      </c>
-      <c r="E11" s="10">
-        <v>1.8</v>
-      </c>
-      <c r="F11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" t="s">
-        <v>243</v>
-      </c>
-      <c r="I11" t="s">
-        <v>253</v>
-      </c>
-      <c r="J11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11">
-        <v>20463877</v>
-      </c>
-      <c r="M11" t="s">
-        <v>241</v>
-      </c>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -2023,67 +2235,59 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
-      </c>
-      <c r="E12" s="6">
-        <v>23.56</v>
+        <v>288</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.25</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>170</v>
       </c>
       <c r="H12" t="s">
-        <v>187</v>
+        <v>72</v>
       </c>
       <c r="I12" t="s">
-        <v>227</v>
+        <v>376</v>
       </c>
       <c r="J12" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12">
-        <v>32225176</v>
-      </c>
-      <c r="M12" t="s">
-        <v>226</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="11">
+        <v>0</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
-        <v>184</v>
-      </c>
-      <c r="E13" s="6">
-        <v>31.13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" t="s">
-        <v>186</v>
-      </c>
-      <c r="I13" t="s">
-        <v>228</v>
-      </c>
-      <c r="J13" t="s">
-        <v>116</v>
-      </c>
-      <c r="K13" t="s">
-        <v>90</v>
-      </c>
-      <c r="L13">
-        <v>32225176</v>
-      </c>
-      <c r="M13" t="s">
-        <v>226</v>
-      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -2093,68 +2297,60 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>192</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0.93600000000000005</v>
+        <v>289</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.25</v>
       </c>
       <c r="F14" t="s">
+        <v>170</v>
+      </c>
+      <c r="H14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" t="s">
+        <v>376</v>
+      </c>
+      <c r="J14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>236</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="F15" t="s">
         <v>67</v>
       </c>
-      <c r="H14" t="s">
-        <v>193</v>
-      </c>
-      <c r="I14" t="s">
-        <v>231</v>
-      </c>
-      <c r="J14" t="s">
-        <v>144</v>
-      </c>
-      <c r="K14" t="s">
-        <v>90</v>
-      </c>
-      <c r="L14">
-        <v>9894006</v>
-      </c>
-      <c r="M14" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
-        <v>0</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="E15" s="8">
-        <v>1</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="K15" s="11" t="s">
+      <c r="H15" t="s">
+        <v>237</v>
+      </c>
+      <c r="I15" t="s">
+        <v>247</v>
+      </c>
+      <c r="J15" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" t="s">
         <v>43</v>
       </c>
-      <c r="L15" s="11">
-        <v>15384040</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>223</v>
+      <c r="L15">
+        <v>20463877</v>
+      </c>
+      <c r="M15" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -2165,67 +2361,63 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>209</v>
-      </c>
-      <c r="E16" s="8">
-        <v>0.6</v>
+        <v>183</v>
+      </c>
+      <c r="E16" s="6">
+        <v>23.56</v>
       </c>
       <c r="F16" t="s">
         <v>67</v>
       </c>
       <c r="H16" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="I16" t="s">
-        <v>388</v>
+        <v>223</v>
       </c>
       <c r="J16" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="K16" t="s">
-        <v>385</v>
-      </c>
-      <c r="L16" t="s">
-        <v>386</v>
+        <v>43</v>
+      </c>
+      <c r="L16">
+        <v>32225176</v>
       </c>
       <c r="M16" t="s">
-        <v>387</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="A17" s="13">
+        <v>1</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D17" t="s">
-        <v>196</v>
-      </c>
-      <c r="E17" s="8">
-        <v>14</v>
-      </c>
-      <c r="F17" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" t="s">
-        <v>200</v>
-      </c>
-      <c r="I17" t="s">
-        <v>233</v>
-      </c>
-      <c r="J17" t="s">
-        <v>161</v>
-      </c>
-      <c r="K17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17">
-        <v>15384040</v>
-      </c>
-      <c r="M17" t="s">
-        <v>223</v>
-      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="E17" s="6">
+        <v>150</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
@@ -2236,32 +2428,30 @@
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="E18" s="10">
-        <v>3.7999999999999999E-2</v>
+        <v>184</v>
+      </c>
+      <c r="E18" s="15">
+        <v>31.13</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="G18" s="11"/>
       <c r="H18" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>238</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="I18" s="11"/>
       <c r="J18" s="11" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>236</v>
+        <v>90</v>
       </c>
       <c r="L18" s="11">
-        <v>15384040</v>
+        <v>32225176</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -2272,31 +2462,31 @@
         <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" s="10">
-        <v>0.6</v>
+        <v>455</v>
+      </c>
+      <c r="E19" s="6">
+        <v>4670</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="H19" t="s">
-        <v>201</v>
+        <v>456</v>
       </c>
       <c r="I19" t="s">
-        <v>388</v>
+        <v>457</v>
       </c>
       <c r="J19" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="K19" t="s">
-        <v>385</v>
-      </c>
-      <c r="L19" t="s">
-        <v>386</v>
+        <v>43</v>
+      </c>
+      <c r="L19">
+        <v>32225176</v>
       </c>
       <c r="M19" t="s">
-        <v>387</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2307,31 +2497,31 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>198</v>
-      </c>
-      <c r="E20" s="10">
-        <v>10000</v>
+        <v>190</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0.93600000000000005</v>
       </c>
       <c r="F20" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="H20" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="I20" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="J20" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="K20" t="s">
-        <v>236</v>
+        <v>90</v>
       </c>
       <c r="L20">
-        <v>15384040</v>
+        <v>9894006</v>
       </c>
       <c r="M20" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2343,32 +2533,32 @@
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="E21" s="10">
-        <v>0.14000000000000001</v>
+        <v>414</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>67</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>236</v>
+        <v>43</v>
       </c>
       <c r="L21" s="11">
         <v>15384040</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -2379,31 +2569,31 @@
         <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>217</v>
-      </c>
-      <c r="E22" s="10">
-        <v>1</v>
+        <v>414</v>
+      </c>
+      <c r="E22" s="8">
+        <v>2</v>
       </c>
       <c r="F22" t="s">
         <v>67</v>
       </c>
       <c r="H22" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="I22" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="J22" t="s">
         <v>161</v>
       </c>
       <c r="K22" t="s">
-        <v>236</v>
+        <v>377</v>
       </c>
       <c r="L22" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="M22" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2414,66 +2604,68 @@
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>199</v>
-      </c>
-      <c r="E23" s="6">
-        <v>0.17</v>
+        <v>194</v>
+      </c>
+      <c r="E23" s="8">
+        <v>14</v>
       </c>
       <c r="F23" t="s">
         <v>67</v>
       </c>
       <c r="H23" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J23" t="s">
         <v>161</v>
       </c>
       <c r="K23" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="L23">
-        <v>32182409</v>
+        <v>15384040</v>
       </c>
       <c r="M23" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="A24" s="11">
+        <v>0</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D24" t="s">
-        <v>389</v>
-      </c>
-      <c r="E24" s="6">
-        <v>11900</v>
-      </c>
-      <c r="F24" t="s">
-        <v>265</v>
-      </c>
-      <c r="H24" t="s">
-        <v>390</v>
-      </c>
-      <c r="I24" t="s">
-        <v>391</v>
-      </c>
-      <c r="J24" t="s">
-        <v>116</v>
-      </c>
-      <c r="K24" t="s">
-        <v>90</v>
-      </c>
-      <c r="L24">
-        <v>7103258</v>
-      </c>
-      <c r="M24" t="s">
-        <v>219</v>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E24" s="10">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="L24" s="11">
+        <v>15384040</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -2484,29 +2676,476 @@
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>405</v>
-      </c>
-      <c r="E25" s="6">
-        <v>0.17</v>
+        <v>195</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0.5</v>
       </c>
       <c r="F25" t="s">
         <v>67</v>
       </c>
       <c r="H25" t="s">
-        <v>406</v>
+        <v>199</v>
       </c>
       <c r="I25" t="s">
-        <v>407</v>
+        <v>380</v>
       </c>
       <c r="J25" t="s">
         <v>161</v>
       </c>
       <c r="K25" t="s">
+        <v>377</v>
+      </c>
+      <c r="L25" t="s">
+        <v>378</v>
+      </c>
+      <c r="M25" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" s="10">
+        <v>9992</v>
+      </c>
+      <c r="F26" t="s">
+        <v>145</v>
+      </c>
+      <c r="H26" t="s">
+        <v>200</v>
+      </c>
+      <c r="I26" t="s">
+        <v>408</v>
+      </c>
+      <c r="J26" t="s">
+        <v>161</v>
+      </c>
+      <c r="K26" t="s">
+        <v>231</v>
+      </c>
+      <c r="L26">
+        <v>15384040</v>
+      </c>
+      <c r="M26" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>0</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="L27" s="11">
+        <v>15384040</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" t="s">
+        <v>213</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0.39</v>
+      </c>
+      <c r="F28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" t="s">
+        <v>214</v>
+      </c>
+      <c r="I28" t="s">
+        <v>380</v>
+      </c>
+      <c r="J28" t="s">
+        <v>161</v>
+      </c>
+      <c r="K28" t="s">
+        <v>231</v>
+      </c>
+      <c r="L28" t="s">
+        <v>378</v>
+      </c>
+      <c r="M28" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" t="s">
+        <v>201</v>
+      </c>
+      <c r="I29" t="s">
+        <v>225</v>
+      </c>
+      <c r="J29" t="s">
+        <v>161</v>
+      </c>
+      <c r="K29" t="s">
+        <v>90</v>
+      </c>
+      <c r="L29">
+        <v>32182409</v>
+      </c>
+      <c r="M29" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" t="s">
+        <v>381</v>
+      </c>
+      <c r="E30" s="6">
+        <v>11900</v>
+      </c>
+      <c r="F30" t="s">
+        <v>259</v>
+      </c>
+      <c r="H30" t="s">
+        <v>382</v>
+      </c>
+      <c r="I30" t="s">
+        <v>383</v>
+      </c>
+      <c r="J30" t="s">
+        <v>116</v>
+      </c>
+      <c r="K30" t="s">
+        <v>90</v>
+      </c>
+      <c r="L30">
+        <v>7103258</v>
+      </c>
+      <c r="M30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" t="s">
+        <v>397</v>
+      </c>
+      <c r="E31" s="6">
+        <v>17</v>
+      </c>
+      <c r="F31" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" t="s">
+        <v>398</v>
+      </c>
+      <c r="I31" t="s">
+        <v>399</v>
+      </c>
+      <c r="J31" t="s">
+        <v>161</v>
+      </c>
+      <c r="K31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H56">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="13">
+        <v>1</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="E32" s="14">
+        <v>0</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="13">
+        <v>1</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="E33" s="13">
+        <v>50</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="13">
+        <v>1</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="E34" s="14">
+        <v>190</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
+        <v>1</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="E35" s="14">
+        <v>700</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="13">
+        <v>1</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="E36" s="14">
+        <v>5</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="K36" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="13">
+        <v>1</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="E37" s="14">
+        <v>14300</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L37" s="13">
+        <v>32404477</v>
+      </c>
+      <c r="M37" s="13"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="13">
+        <v>1</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="E38" s="14">
+        <v>941000</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="K38" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L38" s="13">
+        <v>15358653</v>
+      </c>
+      <c r="M38" s="13"/>
+    </row>
+    <row r="62" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H62">
         <v>44</v>
       </c>
     </row>
@@ -2518,10 +3157,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2613,20 +3255,20 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D5" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="G5" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="I5" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="K5" t="s">
         <v>181</v>
@@ -2637,17 +3279,17 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D6" t="s">
         <v>180</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G6" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="I6" t="s">
         <v>185</v>
@@ -2661,19 +3303,19 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D7" t="s">
         <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="G7" t="s">
         <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="K7" t="s">
         <v>116</v>
@@ -2684,67 +3326,77 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D8" t="s">
         <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="G8" t="s">
         <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="K8" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D9" t="s">
-        <v>263</v>
-      </c>
-      <c r="F9" t="s">
-        <v>264</v>
-      </c>
-      <c r="G9" t="s">
-        <v>265</v>
-      </c>
-      <c r="I9" t="s">
-        <v>266</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="A9" s="13">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>254</v>
-      </c>
-      <c r="D10" t="s">
-        <v>267</v>
-      </c>
-      <c r="F10" t="s">
-        <v>268</v>
-      </c>
-      <c r="G10" t="s">
-        <v>265</v>
-      </c>
-      <c r="I10" t="s">
-        <v>269</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="A10" s="13">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="K10" s="13" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2753,22 +3405,22 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D11" t="s">
-        <v>328</v>
+        <v>257</v>
       </c>
       <c r="F11" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="G11" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I11" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K11" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2776,22 +3428,22 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="F12" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="G12" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I12" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="K12" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2799,19 +3451,19 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D13" t="s">
-        <v>276</v>
+        <v>320</v>
       </c>
       <c r="F13" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="G13" t="s">
+        <v>259</v>
+      </c>
+      <c r="I13" t="s">
         <v>265</v>
-      </c>
-      <c r="I13" t="s">
-        <v>277</v>
       </c>
       <c r="K13" t="s">
         <v>144</v>
@@ -2822,22 +3474,22 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D14" t="s">
-        <v>367</v>
+        <v>266</v>
       </c>
       <c r="F14" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="G14" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I14" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="K14" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2845,22 +3497,22 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D15" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="F15" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="G15" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I15" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="K15" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2868,19 +3520,19 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D16" t="s">
-        <v>279</v>
+        <v>359</v>
       </c>
       <c r="F16" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="G16" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I16" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="K16" t="s">
         <v>161</v>
@@ -2891,19 +3543,19 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D17" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="F17" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="G17" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I17" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="K17" t="s">
         <v>161</v>
@@ -2914,45 +3566,49 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D18" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="F18" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="G18" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="I18" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="K18" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>254</v>
-      </c>
-      <c r="D19" t="s">
-        <v>337</v>
-      </c>
-      <c r="F19" t="s">
-        <v>336</v>
-      </c>
-      <c r="G19" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" t="s">
-        <v>338</v>
-      </c>
-      <c r="K19" t="s">
-        <v>65</v>
+      <c r="A19" s="13">
+        <v>1</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2960,45 +3616,49 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>248</v>
+      </c>
+      <c r="D20" t="s">
+        <v>280</v>
+      </c>
+      <c r="F20" t="s">
+        <v>281</v>
+      </c>
+      <c r="G20" t="s">
+        <v>259</v>
+      </c>
+      <c r="I20" t="s">
+        <v>282</v>
+      </c>
+      <c r="K20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
+        <v>0</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="D20" t="s">
-        <v>339</v>
-      </c>
-      <c r="F20" t="s">
-        <v>340</v>
-      </c>
-      <c r="G20" t="s">
-        <v>89</v>
-      </c>
-      <c r="I20" t="s">
-        <v>341</v>
-      </c>
-      <c r="K20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>254</v>
-      </c>
-      <c r="D21" t="s">
-        <v>342</v>
-      </c>
-      <c r="F21" t="s">
-        <v>343</v>
-      </c>
-      <c r="G21" t="s">
-        <v>89</v>
-      </c>
-      <c r="I21" t="s">
-        <v>344</v>
-      </c>
-      <c r="K21" t="s">
-        <v>65</v>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -3006,22 +3666,22 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D22" t="s">
-        <v>346</v>
+        <v>470</v>
       </c>
       <c r="F22" t="s">
-        <v>345</v>
+        <v>471</v>
       </c>
       <c r="G22" t="s">
-        <v>89</v>
+        <v>250</v>
       </c>
       <c r="I22" t="s">
-        <v>347</v>
+        <v>469</v>
       </c>
       <c r="K22" t="s">
-        <v>65</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -3029,22 +3689,22 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D23" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="F23" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="G23" t="s">
-        <v>265</v>
+        <v>40</v>
       </c>
       <c r="I23" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="K23" t="s">
-        <v>351</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -3052,22 +3712,22 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D24" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
       <c r="F24" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
       <c r="G24" t="s">
-        <v>265</v>
+        <v>89</v>
       </c>
       <c r="I24" t="s">
-        <v>354</v>
+        <v>333</v>
       </c>
       <c r="K24" t="s">
-        <v>351</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -3075,22 +3735,22 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D25" t="s">
-        <v>355</v>
+        <v>334</v>
       </c>
       <c r="F25" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="G25" t="s">
-        <v>265</v>
+        <v>89</v>
       </c>
       <c r="I25" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="K25" t="s">
-        <v>351</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -3098,22 +3758,22 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D26" t="s">
-        <v>363</v>
+        <v>338</v>
       </c>
       <c r="F26" t="s">
-        <v>364</v>
+        <v>337</v>
       </c>
       <c r="G26" t="s">
-        <v>265</v>
+        <v>89</v>
       </c>
       <c r="I26" t="s">
-        <v>365</v>
+        <v>339</v>
       </c>
       <c r="K26" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -3121,22 +3781,22 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D27" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
       <c r="F27" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="G27" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I27" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="K27" t="s">
-        <v>75</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -3144,22 +3804,22 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D28" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="F28" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="G28" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I28" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="K28" t="s">
-        <v>75</v>
+        <v>343</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -3167,22 +3827,22 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D29" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="F29" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>259</v>
       </c>
       <c r="I29" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="K29" t="s">
-        <v>116</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -3190,22 +3850,22 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D30" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="F30" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>259</v>
       </c>
       <c r="I30" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="K30" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -3213,22 +3873,22 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D31" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F31" t="s">
-        <v>374</v>
+        <v>353</v>
       </c>
       <c r="G31" t="s">
-        <v>89</v>
+        <v>259</v>
       </c>
       <c r="I31" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="K31" t="s">
-        <v>161</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -3236,21 +3896,194 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D32" t="s">
-        <v>408</v>
+        <v>351</v>
       </c>
       <c r="F32" t="s">
-        <v>409</v>
+        <v>350</v>
       </c>
       <c r="G32" t="s">
+        <v>259</v>
+      </c>
+      <c r="I32" t="s">
+        <v>354</v>
+      </c>
+      <c r="K32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>248</v>
+      </c>
+      <c r="D33" t="s">
+        <v>361</v>
+      </c>
+      <c r="F33" t="s">
+        <v>360</v>
+      </c>
+      <c r="G33" t="s">
         <v>89</v>
       </c>
-      <c r="I32" t="s">
-        <v>410</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="I33" t="s">
+        <v>362</v>
+      </c>
+      <c r="K33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>248</v>
+      </c>
+      <c r="D34" t="s">
+        <v>363</v>
+      </c>
+      <c r="F34" t="s">
+        <v>364</v>
+      </c>
+      <c r="G34" t="s">
+        <v>89</v>
+      </c>
+      <c r="I34" t="s">
+        <v>362</v>
+      </c>
+      <c r="K34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>248</v>
+      </c>
+      <c r="D35" t="s">
+        <v>365</v>
+      </c>
+      <c r="F35" t="s">
+        <v>366</v>
+      </c>
+      <c r="G35" t="s">
+        <v>89</v>
+      </c>
+      <c r="I35" t="s">
+        <v>362</v>
+      </c>
+      <c r="K35" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="11">
+        <v>0</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>248</v>
+      </c>
+      <c r="D37" t="s">
+        <v>400</v>
+      </c>
+      <c r="F37" t="s">
+        <v>424</v>
+      </c>
+      <c r="G37" t="s">
+        <v>89</v>
+      </c>
+      <c r="I37" t="s">
+        <v>401</v>
+      </c>
+      <c r="K37" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="13">
+        <v>1</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="13">
+        <v>1</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3264,7 +4097,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3401,46 +4234,52 @@
         <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="J6" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="L6" t="s">
         <v>90</v>
       </c>
       <c r="M6" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="N6" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="11">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
-        <v>296</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="E7" s="11">
         <v>0.26700000000000002</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="J7" t="s">
-        <v>221</v>
-      </c>
-      <c r="M7" t="s">
-        <v>221</v>
-      </c>
+      <c r="J7" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -3456,13 +4295,13 @@
         <v>1.33E-12</v>
       </c>
       <c r="G8" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="I8" t="s">
         <v>85</v>
       </c>
       <c r="J8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="L8" t="s">
         <v>90</v>
@@ -3471,7 +4310,7 @@
         <v>7103258</v>
       </c>
       <c r="N8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3481,10 +4320,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3494,7 +4333,7 @@
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
@@ -3618,10 +4457,10 @@
         <v>78</v>
       </c>
       <c r="K5" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="L5" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="M5" t="s">
         <v>65</v>
@@ -3633,7 +4472,7 @@
         <v>7103258</v>
       </c>
       <c r="P5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -3711,10 +4550,10 @@
         <v>78</v>
       </c>
       <c r="K8" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="L8" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="M8" t="s">
         <v>65</v>
@@ -3726,7 +4565,7 @@
         <v>7103258</v>
       </c>
       <c r="P8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -3755,7 +4594,7 @@
         <v>176</v>
       </c>
       <c r="L9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="M9" t="s">
         <v>116</v>
@@ -3772,7 +4611,7 @@
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E10" s="9">
         <v>615</v>
@@ -3793,7 +4632,7 @@
         <v>176</v>
       </c>
       <c r="L10" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="M10" t="s">
         <v>116</v>
@@ -3912,7 +4751,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>190</v>
+        <v>405</v>
       </c>
       <c r="M14" t="s">
         <v>144</v>
@@ -3926,7 +4765,7 @@
         <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -3941,7 +4780,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="M15" t="s">
         <v>161</v>
@@ -3955,7 +4794,7 @@
         <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -3970,13 +4809,13 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="M16" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3999,13 +4838,13 @@
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>191</v>
+        <v>404</v>
       </c>
       <c r="M17" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -4013,7 +4852,7 @@
         <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -4028,13 +4867,13 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M18" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -4045,7 +4884,7 @@
         <v>75</v>
       </c>
       <c r="E19" s="5">
-        <v>2E-3</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="G19" t="s">
         <v>145</v>
@@ -4060,7 +4899,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -4068,7 +4907,7 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -4080,10 +4919,86 @@
         <v>78</v>
       </c>
       <c r="K20" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="M20" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="13">
+        <v>1</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="13">
+        <v>1</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13" t="s">
+        <v>453</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13">
+        <v>32350462</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -4094,10 +5009,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4222,7 +5140,7 @@
         <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="F6" t="s">
         <v>53</v>
@@ -4248,7 +5166,7 @@
         <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="F7" t="s">
         <v>53</v>
@@ -4375,10 +5293,10 @@
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E12" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F12" t="s">
         <v>92</v>
@@ -4387,7 +5305,7 @@
         <v>94</v>
       </c>
       <c r="I12" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="K12" t="s">
         <v>116</v>
@@ -4404,7 +5322,7 @@
         <v>97</v>
       </c>
       <c r="E13" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="F13" t="s">
         <v>92</v>
@@ -4446,28 +5364,31 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="11">
+        <v>0</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G15" t="s">
-        <v>378</v>
-      </c>
-      <c r="I15" t="s">
-        <v>397</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="G15" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4479,19 +5400,19 @@
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E16" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F16" t="s">
         <v>92</v>
       </c>
       <c r="G16" t="s">
-        <v>108</v>
+        <v>418</v>
       </c>
       <c r="I16" t="s">
-        <v>109</v>
+        <v>419</v>
       </c>
       <c r="K16" t="s">
         <v>116</v>
@@ -4505,19 +5426,19 @@
         <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F17" t="s">
         <v>92</v>
       </c>
       <c r="G17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K17" t="s">
         <v>116</v>
@@ -4531,22 +5452,22 @@
         <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E18" t="s">
-        <v>164</v>
+        <v>111</v>
       </c>
       <c r="F18" t="s">
         <v>92</v>
       </c>
       <c r="G18" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="I18" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="K18" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -4557,19 +5478,19 @@
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>246</v>
+        <v>117</v>
       </c>
       <c r="E19" t="s">
-        <v>247</v>
+        <v>164</v>
       </c>
       <c r="F19" t="s">
         <v>92</v>
       </c>
       <c r="G19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I19" t="s">
-        <v>248</v>
+        <v>146</v>
       </c>
       <c r="K19" t="s">
         <v>144</v>
@@ -4583,19 +5504,19 @@
         <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>240</v>
       </c>
       <c r="E20" t="s">
-        <v>376</v>
+        <v>241</v>
       </c>
       <c r="F20" t="s">
         <v>92</v>
       </c>
       <c r="G20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I20" t="s">
-        <v>147</v>
+        <v>242</v>
       </c>
       <c r="K20" t="s">
         <v>144</v>
@@ -4609,19 +5530,19 @@
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E21" t="s">
-        <v>132</v>
+        <v>368</v>
       </c>
       <c r="F21" t="s">
         <v>92</v>
       </c>
       <c r="G21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K21" t="s">
         <v>144</v>
@@ -4635,47 +5556,50 @@
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F22" t="s">
         <v>92</v>
       </c>
       <c r="G22" t="s">
-        <v>379</v>
+        <v>128</v>
       </c>
       <c r="I22" t="s">
-        <v>398</v>
+        <v>148</v>
       </c>
       <c r="K22" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="A23" s="11">
+        <v>0</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E23" t="s">
-        <v>136</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G23" t="s">
-        <v>380</v>
-      </c>
-      <c r="I23" t="s">
-        <v>399</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="G23" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4687,108 +5611,102 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F24" t="s">
         <v>92</v>
       </c>
       <c r="G24" t="s">
-        <v>139</v>
+        <v>420</v>
       </c>
       <c r="I24" t="s">
-        <v>138</v>
+        <v>421</v>
       </c>
       <c r="K24" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="12">
-        <v>1</v>
-      </c>
-      <c r="B25" s="12" t="s">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12" t="s">
+      <c r="D25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" t="s">
+        <v>372</v>
+      </c>
+      <c r="I25" t="s">
+        <v>391</v>
+      </c>
+      <c r="K25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" t="s">
+        <v>139</v>
+      </c>
+      <c r="I26" t="s">
+        <v>138</v>
+      </c>
+      <c r="K26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>0</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="12">
-        <v>1</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12" t="s">
-        <v>306</v>
-      </c>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="12">
-        <v>1</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>307</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12" t="s">
+      <c r="J27" s="11"/>
+      <c r="K27" s="11" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4801,20 +5719,20 @@
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12" t="s">
-        <v>143</v>
+        <v>300</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12" t="s">
@@ -4830,24 +5748,24 @@
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>83</v>
+        <v>301</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>311</v>
+        <v>131</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -4859,24 +5777,24 @@
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12" t="s">
-        <v>309</v>
+        <v>140</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>313</v>
+        <v>141</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>314</v>
+        <v>142</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12" t="s">
-        <v>315</v>
+        <v>143</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -4888,20 +5806,20 @@
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>377</v>
+        <v>83</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12" t="s">
@@ -4917,20 +5835,20 @@
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12" t="s">
-        <v>123</v>
+        <v>303</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12" t="s">
@@ -4946,20 +5864,20 @@
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>320</v>
+        <v>369</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>381</v>
+        <v>310</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="12" t="s">
-        <v>400</v>
+        <v>311</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12" t="s">
@@ -4975,20 +5893,20 @@
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
-        <v>310</v>
+        <v>123</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>321</v>
+        <v>416</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="12" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12" t="s">
@@ -4996,109 +5914,118 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="12">
-        <v>1</v>
-      </c>
-      <c r="B35" s="12" t="s">
+      <c r="A35" s="11">
+        <v>0</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12" t="s">
+      <c r="C35" s="11"/>
+      <c r="D35" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="12">
+        <v>1</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="12">
+        <v>1</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="12">
+        <v>1</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E38" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F38" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G38" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12" t="s">
+      <c r="H38" s="12"/>
+      <c r="I38" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" t="s">
-        <v>154</v>
-      </c>
-      <c r="E36" t="s">
-        <v>235</v>
-      </c>
-      <c r="F36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G36" t="s">
-        <v>155</v>
-      </c>
-      <c r="I36" t="s">
-        <v>156</v>
-      </c>
-      <c r="K36" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" t="s">
-        <v>213</v>
-      </c>
-      <c r="E37" t="s">
-        <v>214</v>
-      </c>
-      <c r="F37" t="s">
-        <v>92</v>
-      </c>
-      <c r="G37" t="s">
-        <v>215</v>
-      </c>
-      <c r="I37" t="s">
-        <v>216</v>
-      </c>
-      <c r="K37" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" t="s">
-        <v>157</v>
-      </c>
-      <c r="E38" t="s">
-        <v>212</v>
-      </c>
-      <c r="F38" t="s">
-        <v>92</v>
-      </c>
-      <c r="G38" t="s">
-        <v>204</v>
-      </c>
-      <c r="I38" t="s">
-        <v>205</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="J38" s="12"/>
+      <c r="K38" s="12" t="s">
         <v>161</v>
       </c>
     </row>
@@ -5110,19 +6037,19 @@
         <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E39" t="s">
-        <v>162</v>
+        <v>230</v>
       </c>
       <c r="F39" t="s">
         <v>92</v>
       </c>
       <c r="G39" t="s">
-        <v>382</v>
+        <v>155</v>
       </c>
       <c r="I39" t="s">
-        <v>401</v>
+        <v>156</v>
       </c>
       <c r="K39" t="s">
         <v>161</v>
@@ -5137,20 +6064,20 @@
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
-        <v>159</v>
+        <v>209</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>92</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>383</v>
+        <v>211</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="11" t="s">
-        <v>160</v>
+        <v>212</v>
       </c>
       <c r="J40" s="11"/>
       <c r="K40" s="11" t="s">
@@ -5165,47 +6092,50 @@
         <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>159</v>
+        <v>209</v>
       </c>
       <c r="E41" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
       <c r="F41" t="s">
         <v>92</v>
       </c>
       <c r="G41" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="I41" t="s">
-        <v>393</v>
+        <v>212</v>
       </c>
       <c r="K41" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="A42" s="11">
+        <v>0</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D42" t="s">
-        <v>52</v>
-      </c>
-      <c r="E42" t="s">
-        <v>82</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="C42" s="11"/>
+      <c r="D42" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G42" t="s">
-        <v>165</v>
-      </c>
-      <c r="I42" t="s">
-        <v>166</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="G42" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11" t="s">
         <v>161</v>
       </c>
     </row>
@@ -5217,26 +6147,188 @@
         <v>35</v>
       </c>
       <c r="D43" t="s">
-        <v>394</v>
+        <v>157</v>
       </c>
       <c r="E43" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="F43" t="s">
         <v>92</v>
       </c>
       <c r="G43" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="I43" t="s">
-        <v>396</v>
+        <v>203</v>
       </c>
       <c r="K43" t="s">
         <v>161</v>
       </c>
     </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" t="s">
+        <v>162</v>
+      </c>
+      <c r="F44" t="s">
+        <v>92</v>
+      </c>
+      <c r="G44" t="s">
+        <v>374</v>
+      </c>
+      <c r="I44" t="s">
+        <v>393</v>
+      </c>
+      <c r="K44" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="13">
+        <v>1</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="11">
+        <v>0</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" t="s">
+        <v>159</v>
+      </c>
+      <c r="E47" t="s">
+        <v>163</v>
+      </c>
+      <c r="F47" t="s">
+        <v>92</v>
+      </c>
+      <c r="G47" t="s">
+        <v>384</v>
+      </c>
+      <c r="I47" t="s">
+        <v>385</v>
+      </c>
+      <c r="K47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" t="s">
+        <v>165</v>
+      </c>
+      <c r="I48" t="s">
+        <v>166</v>
+      </c>
+      <c r="K48" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" t="s">
+        <v>386</v>
+      </c>
+      <c r="E49" t="s">
+        <v>396</v>
+      </c>
+      <c r="F49" t="s">
+        <v>92</v>
+      </c>
+      <c r="G49" t="s">
+        <v>387</v>
+      </c>
+      <c r="I49" t="s">
+        <v>388</v>
+      </c>
+      <c r="K49" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A4:K43" xr:uid="{6674B1C7-2B72-4099-8A9D-5016CD5D9EBF}"/>
+  <autoFilter ref="A4:K49" xr:uid="{6674B1C7-2B72-4099-8A9D-5016CD5D9EBF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updates after unit checking
</commit_message>
<xml_diff>
--- a/src/Cov19_life_cycle/cov19_life_cycle.xlsx
+++ b/src/Cov19_life_cycle/cov19_life_cycle.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Const" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="477">
   <si>
     <t>on</t>
   </si>
@@ -541,9 +541,6 @@
     <t>concentration of  COV (SARS-CoV-2 virus)</t>
   </si>
   <si>
-    <t>1/pM/h</t>
-  </si>
-  <si>
     <t>ACE2_pc</t>
   </si>
   <si>
@@ -763,9 +760,6 @@
     <t>k_shed_ace2_pc*ACE2_pc_hs_ss/PC_hs_ss/Vol_pc/Vol_alv/kcell_to_cell</t>
   </si>
   <si>
-    <t>pM/h/cell</t>
-  </si>
-  <si>
     <t>L/cell</t>
   </si>
   <si>
@@ -1363,9 +1357,6 @@
     <t>Hill coefficient of IR effect on vPC apoptosis</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1 + switch_ir*Emax_ir_apo*(t - T_sw_ir)^n_ir/((T_sw_ir + ET50_ir)^n_ir + (t - T_sw_ir)^n_ir)</t>
-  </si>
-  <si>
     <t>kbase_apo_vpc</t>
   </si>
   <si>
@@ -1420,9 +1411,6 @@
     <t>concentration of anti-Spike attibodies</t>
   </si>
   <si>
-    <t xml:space="preserve"> switch_ir*anti_Ab_max*(t - T_sw_ir)^n_ir/((T_sw_ir + ET50_ir)^n_ir + (t - T_sw_ir)^n_ir)</t>
-  </si>
-  <si>
     <t>hill like expression describes general kinetic pattern observed for Spike specific IgG and IgM in [32350462]</t>
   </si>
   <si>
@@ -1441,9 +1429,6 @@
     <t>COV_num_sputum_ml</t>
   </si>
   <si>
-    <t>sputum_dilution_coef*(COV + COV_RNA)*Vol_alv*NA_pmole/1000</t>
-  </si>
-  <si>
     <t>sputum_dilution_coef</t>
   </si>
   <si>
@@ -1454,6 +1439,27 @@
   </si>
   <si>
     <t>averaged between type I and II pneumocytes (moved to Const)</t>
+  </si>
+  <si>
+    <t>pM/h</t>
+  </si>
+  <si>
+    <t>1/pmole/h</t>
+  </si>
+  <si>
+    <t>L_to_mL</t>
+  </si>
+  <si>
+    <t>mL/L</t>
+  </si>
+  <si>
+    <t>sputum_dilution_coef*(COV + COV_RNA)*NA_pmole/L_to_mL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 + switch_ir*Emax_ir_apo*(t/T_sw_ir - 1)^n_ir/((1 + ET50_ir/T_sw_ir)^n_ir + (t/T_sw_ir - 1)^n_ir)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> switch_ir*anti_Ab_max*(t/T_sw_ir - 1)^n_ir/((1 + ET50_ir/T_sw_ir)^n_ir + (t/T_sw_ir - 1)^n_ir)</t>
   </si>
 </sst>
 </file>
@@ -1558,7 +1564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1575,6 +1581,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1885,7 +1892,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H40" sqref="H40"/>
+      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1989,13 +1996,13 @@
         <v>1000</v>
       </c>
       <c r="F5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K5" t="s">
         <v>43</v>
@@ -2009,19 +2016,19 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E6" s="6">
         <v>602000000000</v>
       </c>
       <c r="F6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K6" t="s">
         <v>43</v>
@@ -2036,7 +2043,7 @@
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E7" s="6">
         <v>0.1</v>
@@ -2046,17 +2053,17 @@
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K7" s="13" t="s">
         <v>43</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="M7" s="13"/>
     </row>
@@ -2080,7 +2087,7 @@
         <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J8" t="s">
         <v>65</v>
@@ -2089,7 +2096,7 @@
         <v>90</v>
       </c>
       <c r="L8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -2114,7 +2121,7 @@
         <v>103</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>65</v>
@@ -2123,7 +2130,7 @@
         <v>90</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M9" s="11"/>
     </row>
@@ -2135,7 +2142,7 @@
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E10" s="6">
         <v>8.1999999999999998E-4</v>
@@ -2147,7 +2154,7 @@
         <v>103</v>
       </c>
       <c r="I10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J10" t="s">
         <v>65</v>
@@ -2156,7 +2163,7 @@
         <v>90</v>
       </c>
       <c r="L10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -2168,20 +2175,20 @@
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E11" s="15">
         <v>0.01</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>170</v>
+        <v>471</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11" t="s">
         <v>72</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>65</v>
@@ -2200,25 +2207,25 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E12" s="5">
         <v>0.25</v>
       </c>
       <c r="F12" t="s">
-        <v>170</v>
+        <v>471</v>
       </c>
       <c r="H12" t="s">
         <v>72</v>
       </c>
       <c r="I12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J12" t="s">
         <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -2230,20 +2237,20 @@
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E13" s="15">
         <v>0.01</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>170</v>
+        <v>471</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11" t="s">
         <v>73</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>65</v>
@@ -2262,25 +2269,25 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E14" s="5">
         <v>0.25</v>
       </c>
       <c r="F14" t="s">
-        <v>170</v>
+        <v>471</v>
       </c>
       <c r="H14" t="s">
         <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J14" t="s">
         <v>65</v>
       </c>
       <c r="K14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -2291,7 +2298,7 @@
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E15" s="10">
         <v>1.8</v>
@@ -2300,10 +2307,10 @@
         <v>67</v>
       </c>
       <c r="H15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J15" t="s">
         <v>116</v>
@@ -2315,7 +2322,7 @@
         <v>20463877</v>
       </c>
       <c r="M15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -2326,7 +2333,7 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E16" s="6">
         <v>23.56</v>
@@ -2335,10 +2342,10 @@
         <v>67</v>
       </c>
       <c r="H16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J16" t="s">
         <v>116</v>
@@ -2350,7 +2357,7 @@
         <v>32225176</v>
       </c>
       <c r="M16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
@@ -2362,7 +2369,7 @@
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E17" s="6">
         <v>150</v>
@@ -2372,14 +2379,14 @@
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
@@ -2393,7 +2400,7 @@
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E18" s="15">
         <v>31.13</v>
@@ -2403,7 +2410,7 @@
       </c>
       <c r="G18" s="11"/>
       <c r="H18" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I18" s="11"/>
       <c r="J18" s="11" t="s">
@@ -2416,7 +2423,7 @@
         <v>32225176</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
@@ -2427,7 +2434,7 @@
         <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E19" s="6">
         <v>4670</v>
@@ -2436,10 +2443,10 @@
         <v>145</v>
       </c>
       <c r="H19" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="I19" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="J19" t="s">
         <v>116</v>
@@ -2451,7 +2458,7 @@
         <v>32225176</v>
       </c>
       <c r="M19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
@@ -2462,7 +2469,7 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E20" s="8">
         <v>0.93600000000000005</v>
@@ -2471,10 +2478,10 @@
         <v>67</v>
       </c>
       <c r="H20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J20" t="s">
         <v>144</v>
@@ -2486,7 +2493,7 @@
         <v>9894006</v>
       </c>
       <c r="M20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
@@ -2498,7 +2505,7 @@
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E21" s="8">
         <v>1</v>
@@ -2508,10 +2515,10 @@
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>144</v>
@@ -2523,7 +2530,7 @@
         <v>15384040</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
@@ -2534,7 +2541,7 @@
         <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E22" s="8">
         <v>2</v>
@@ -2543,22 +2550,22 @@
         <v>67</v>
       </c>
       <c r="H22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I22" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J22" t="s">
         <v>161</v>
       </c>
       <c r="K22" t="s">
+        <v>374</v>
+      </c>
+      <c r="L22" t="s">
+        <v>375</v>
+      </c>
+      <c r="M22" t="s">
         <v>376</v>
-      </c>
-      <c r="L22" t="s">
-        <v>377</v>
-      </c>
-      <c r="M22" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
@@ -2569,7 +2576,7 @@
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E23" s="8">
         <v>14</v>
@@ -2578,10 +2585,10 @@
         <v>67</v>
       </c>
       <c r="H23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J23" t="s">
         <v>161</v>
@@ -2593,7 +2600,7 @@
         <v>15384040</v>
       </c>
       <c r="M23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
@@ -2605,7 +2612,7 @@
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E24" s="10">
         <v>3.7999999999999999E-2</v>
@@ -2615,22 +2622,22 @@
       </c>
       <c r="G24" s="11"/>
       <c r="H24" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>161</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L24" s="11">
         <v>15384040</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
@@ -2641,7 +2648,7 @@
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E25" s="10">
         <v>0.5</v>
@@ -2650,22 +2657,22 @@
         <v>67</v>
       </c>
       <c r="H25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I25" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J25" t="s">
         <v>161</v>
       </c>
       <c r="K25" t="s">
+        <v>374</v>
+      </c>
+      <c r="L25" t="s">
+        <v>375</v>
+      </c>
+      <c r="M25" t="s">
         <v>376</v>
-      </c>
-      <c r="L25" t="s">
-        <v>377</v>
-      </c>
-      <c r="M25" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
@@ -2676,7 +2683,7 @@
         <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E26" s="10">
         <v>9992</v>
@@ -2685,22 +2692,22 @@
         <v>145</v>
       </c>
       <c r="H26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I26" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="J26" t="s">
         <v>161</v>
       </c>
       <c r="K26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L26">
         <v>15384040</v>
       </c>
       <c r="M26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
@@ -2712,7 +2719,7 @@
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E27" s="10">
         <v>0.14000000000000001</v>
@@ -2722,22 +2729,22 @@
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J27" s="11" t="s">
         <v>161</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L27" s="11">
         <v>15384040</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
@@ -2748,7 +2755,7 @@
         <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E28" s="10">
         <v>0.39</v>
@@ -2757,22 +2764,22 @@
         <v>67</v>
       </c>
       <c r="H28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I28" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J28" t="s">
         <v>161</v>
       </c>
       <c r="K28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L28" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M28" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
@@ -2783,7 +2790,7 @@
         <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E29" s="6">
         <v>0.17</v>
@@ -2792,10 +2799,10 @@
         <v>67</v>
       </c>
       <c r="H29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J29" t="s">
         <v>161</v>
@@ -2807,7 +2814,7 @@
         <v>32182409</v>
       </c>
       <c r="M29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -2818,19 +2825,19 @@
         <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E30" s="6">
         <v>11900</v>
       </c>
       <c r="F30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H30" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I30" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="J30" t="s">
         <v>116</v>
@@ -2842,7 +2849,7 @@
         <v>7103258</v>
       </c>
       <c r="M30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -2853,7 +2860,7 @@
         <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E31" s="6">
         <v>17</v>
@@ -2862,10 +2869,10 @@
         <v>67</v>
       </c>
       <c r="H31" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I31" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J31" t="s">
         <v>161</v>
@@ -2883,7 +2890,7 @@
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E32" s="14">
         <v>0</v>
@@ -2893,13 +2900,13 @@
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I32" s="13" t="s">
         <v>42</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K32" s="13" t="s">
         <v>42</v>
@@ -2916,23 +2923,23 @@
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E33" s="13">
         <v>50</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="I33" s="13" t="s">
         <v>42</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K33" s="13" t="s">
         <v>42</v>
@@ -2949,23 +2956,23 @@
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E34" s="14">
         <v>190</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="I34" s="13" t="s">
         <v>42</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K34" s="13" t="s">
         <v>42</v>
@@ -2982,7 +2989,7 @@
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E35" s="14">
         <v>700</v>
@@ -2992,13 +2999,13 @@
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I35" s="13" t="s">
         <v>42</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K35" s="13" t="s">
         <v>42</v>
@@ -3015,7 +3022,7 @@
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E36" s="14">
         <v>5</v>
@@ -3025,13 +3032,13 @@
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="I36" s="13" t="s">
         <v>42</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K36" s="13" t="s">
         <v>42</v>
@@ -3048,7 +3055,7 @@
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="E37" s="14">
         <v>14300</v>
@@ -3058,10 +3065,10 @@
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="J37" s="13" t="s">
         <v>161</v>
@@ -3083,7 +3090,7 @@
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="E38" s="14">
         <v>941000</v>
@@ -3093,13 +3100,13 @@
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="13" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K38" s="13" t="s">
         <v>42</v>
@@ -3124,14 +3131,14 @@
         <v>1.33E-12</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="12" t="s">
         <v>85</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="J39" s="12"/>
       <c r="K39" s="12" t="s">
@@ -3141,11 +3148,29 @@
         <v>7103258</v>
       </c>
       <c r="M39" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N39" s="12"/>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A40" s="12">
+        <v>1</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="E40" s="16">
+        <v>1000</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="62" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H62">
@@ -3166,7 +3191,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3258,23 +3283,23 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" t="s">
+        <v>322</v>
+      </c>
+      <c r="G5" t="s">
+        <v>323</v>
+      </c>
+      <c r="I5" t="s">
         <v>324</v>
       </c>
-      <c r="G5" t="s">
-        <v>325</v>
-      </c>
-      <c r="I5" t="s">
-        <v>326</v>
-      </c>
       <c r="K5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -3282,20 +3307,20 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G6" t="s">
-        <v>244</v>
+        <v>470</v>
       </c>
       <c r="I6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K6" t="s">
         <v>116</v>
@@ -3306,19 +3331,19 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D7" t="s">
         <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G7" t="s">
         <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K7" t="s">
         <v>116</v>
@@ -3329,19 +3354,19 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D8" t="s">
         <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G8" t="s">
         <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="K8" t="s">
         <v>116</v>
@@ -3352,22 +3377,22 @@
         <v>1</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>89</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="13" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13" t="s">
@@ -3379,25 +3404,25 @@
         <v>1</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>145</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>116</v>
@@ -3408,19 +3433,19 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D11" t="s">
+        <v>254</v>
+      </c>
+      <c r="F11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G11" t="s">
         <v>256</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" t="s">
         <v>257</v>
-      </c>
-      <c r="G11" t="s">
-        <v>258</v>
-      </c>
-      <c r="I11" t="s">
-        <v>259</v>
       </c>
       <c r="K11" t="s">
         <v>116</v>
@@ -3431,19 +3456,19 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F12" t="s">
+        <v>259</v>
+      </c>
+      <c r="G12" t="s">
+        <v>256</v>
+      </c>
+      <c r="I12" t="s">
         <v>260</v>
-      </c>
-      <c r="F12" t="s">
-        <v>261</v>
-      </c>
-      <c r="G12" t="s">
-        <v>258</v>
-      </c>
-      <c r="I12" t="s">
-        <v>262</v>
       </c>
       <c r="K12" t="s">
         <v>116</v>
@@ -3454,19 +3479,19 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K13" t="s">
         <v>144</v>
@@ -3477,19 +3502,19 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" t="s">
+        <v>264</v>
+      </c>
+      <c r="G14" t="s">
+        <v>256</v>
+      </c>
+      <c r="I14" t="s">
         <v>265</v>
-      </c>
-      <c r="F14" t="s">
-        <v>266</v>
-      </c>
-      <c r="G14" t="s">
-        <v>258</v>
-      </c>
-      <c r="I14" t="s">
-        <v>267</v>
       </c>
       <c r="K14" t="s">
         <v>144</v>
@@ -3500,19 +3525,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F15" t="s">
+        <v>266</v>
+      </c>
+      <c r="G15" t="s">
+        <v>256</v>
+      </c>
+      <c r="I15" t="s">
         <v>268</v>
-      </c>
-      <c r="G15" t="s">
-        <v>258</v>
-      </c>
-      <c r="I15" t="s">
-        <v>270</v>
       </c>
       <c r="K15" t="s">
         <v>144</v>
@@ -3523,19 +3548,19 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D16" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I16" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K16" t="s">
         <v>161</v>
@@ -3546,19 +3571,19 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D17" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G17" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="K17" t="s">
         <v>161</v>
@@ -3569,19 +3594,19 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="K18" t="s">
         <v>161</v>
@@ -3592,22 +3617,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="13" t="s">
@@ -3619,19 +3644,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D20" t="s">
+        <v>277</v>
+      </c>
+      <c r="F20" t="s">
+        <v>278</v>
+      </c>
+      <c r="G20" t="s">
+        <v>256</v>
+      </c>
+      <c r="I20" t="s">
         <v>279</v>
-      </c>
-      <c r="F20" t="s">
-        <v>280</v>
-      </c>
-      <c r="G20" t="s">
-        <v>258</v>
-      </c>
-      <c r="I20" t="s">
-        <v>281</v>
       </c>
       <c r="K20" t="s">
         <v>161</v>
@@ -3642,22 +3667,22 @@
         <v>0</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J21" s="11"/>
       <c r="K21" s="11" t="s">
@@ -3669,19 +3694,19 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>245</v>
+      </c>
+      <c r="D22" t="s">
+        <v>465</v>
+      </c>
+      <c r="F22" t="s">
+        <v>474</v>
+      </c>
+      <c r="G22" t="s">
         <v>247</v>
       </c>
-      <c r="D22" t="s">
-        <v>469</v>
-      </c>
-      <c r="F22" t="s">
-        <v>470</v>
-      </c>
-      <c r="G22" t="s">
-        <v>249</v>
-      </c>
       <c r="I22" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="K22" t="s">
         <v>161</v>
@@ -3692,19 +3717,19 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F23" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G23" t="s">
         <v>40</v>
       </c>
       <c r="I23" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="K23" t="s">
         <v>65</v>
@@ -3715,19 +3740,19 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D24" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F24" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G24" t="s">
         <v>89</v>
       </c>
       <c r="I24" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="K24" t="s">
         <v>65</v>
@@ -3738,19 +3763,19 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D25" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F25" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G25" t="s">
         <v>89</v>
       </c>
       <c r="I25" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="K25" t="s">
         <v>65</v>
@@ -3761,19 +3786,19 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D26" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F26" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G26" t="s">
         <v>89</v>
       </c>
       <c r="I26" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K26" t="s">
         <v>65</v>
@@ -3784,22 +3809,22 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D27" t="s">
+        <v>338</v>
+      </c>
+      <c r="F27" t="s">
+        <v>337</v>
+      </c>
+      <c r="G27" t="s">
+        <v>256</v>
+      </c>
+      <c r="I27" t="s">
+        <v>339</v>
+      </c>
+      <c r="K27" t="s">
         <v>340</v>
-      </c>
-      <c r="F27" t="s">
-        <v>339</v>
-      </c>
-      <c r="G27" t="s">
-        <v>258</v>
-      </c>
-      <c r="I27" t="s">
-        <v>341</v>
-      </c>
-      <c r="K27" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -3807,22 +3832,22 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D28" t="s">
+        <v>341</v>
+      </c>
+      <c r="F28" t="s">
+        <v>342</v>
+      </c>
+      <c r="G28" t="s">
+        <v>256</v>
+      </c>
+      <c r="I28" t="s">
         <v>343</v>
       </c>
-      <c r="F28" t="s">
-        <v>344</v>
-      </c>
-      <c r="G28" t="s">
-        <v>258</v>
-      </c>
-      <c r="I28" t="s">
-        <v>345</v>
-      </c>
       <c r="K28" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -3830,22 +3855,22 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D29" t="s">
+        <v>344</v>
+      </c>
+      <c r="F29" t="s">
+        <v>345</v>
+      </c>
+      <c r="G29" t="s">
+        <v>256</v>
+      </c>
+      <c r="I29" t="s">
         <v>346</v>
       </c>
-      <c r="F29" t="s">
-        <v>347</v>
-      </c>
-      <c r="G29" t="s">
-        <v>258</v>
-      </c>
-      <c r="I29" t="s">
-        <v>348</v>
-      </c>
       <c r="K29" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -3853,19 +3878,19 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D30" t="s">
+        <v>352</v>
+      </c>
+      <c r="F30" t="s">
+        <v>353</v>
+      </c>
+      <c r="G30" t="s">
+        <v>256</v>
+      </c>
+      <c r="I30" t="s">
         <v>354</v>
-      </c>
-      <c r="F30" t="s">
-        <v>355</v>
-      </c>
-      <c r="G30" t="s">
-        <v>258</v>
-      </c>
-      <c r="I30" t="s">
-        <v>356</v>
       </c>
       <c r="K30" t="s">
         <v>75</v>
@@ -3876,19 +3901,19 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D31" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F31" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G31" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I31" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="K31" t="s">
         <v>75</v>
@@ -3899,19 +3924,19 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D32" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F32" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G32" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I32" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K32" t="s">
         <v>75</v>
@@ -3922,19 +3947,19 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D33" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F33" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G33" t="s">
         <v>89</v>
       </c>
       <c r="I33" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="K33" t="s">
         <v>116</v>
@@ -3945,19 +3970,19 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D34" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F34" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G34" t="s">
         <v>89</v>
       </c>
       <c r="I34" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="K34" t="s">
         <v>144</v>
@@ -3968,19 +3993,19 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D35" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F35" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G35" t="s">
         <v>89</v>
       </c>
       <c r="I35" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="K35" t="s">
         <v>161</v>
@@ -3991,22 +4016,22 @@
         <v>0</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>89</v>
       </c>
       <c r="H36" s="11"/>
       <c r="I36" s="11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J36" s="11"/>
       <c r="K36" s="11" t="s">
@@ -4018,19 +4043,19 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D37" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F37" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G37" t="s">
         <v>89</v>
       </c>
       <c r="I37" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K37" t="s">
         <v>161</v>
@@ -4041,22 +4066,22 @@
         <v>1</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E38" s="13"/>
       <c r="F38" s="13" t="s">
-        <v>444</v>
+        <v>475</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>89</v>
       </c>
       <c r="H38" s="13"/>
       <c r="I38" s="13" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J38" s="13"/>
       <c r="K38" s="13" t="s">
@@ -4068,7 +4093,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13" t="s">
@@ -4076,14 +4101,14 @@
       </c>
       <c r="E39" s="13"/>
       <c r="F39" s="13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>67</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="J39" s="13"/>
       <c r="K39" s="13" t="s">
@@ -4099,7 +4124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -4245,19 +4270,19 @@
         <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L6" t="s">
         <v>90</v>
       </c>
       <c r="M6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -4269,7 +4294,7 @@
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E7" s="11">
         <v>0.26700000000000002</v>
@@ -4283,12 +4308,12 @@
         <v>87</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N7" s="11"/>
     </row>
@@ -4308,14 +4333,14 @@
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
         <v>85</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11" t="s">
@@ -4325,7 +4350,7 @@
         <v>7103258</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4337,8 +4362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4472,10 +4497,10 @@
         <v>78</v>
       </c>
       <c r="K5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="L5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M5" t="s">
         <v>65</v>
@@ -4487,7 +4512,7 @@
         <v>7103258</v>
       </c>
       <c r="P5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
@@ -4565,10 +4590,10 @@
         <v>78</v>
       </c>
       <c r="K8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="L8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M8" t="s">
         <v>65</v>
@@ -4580,7 +4605,7 @@
         <v>7103258</v>
       </c>
       <c r="P8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
@@ -4591,13 +4616,13 @@
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E9" s="9">
         <v>615</v>
       </c>
       <c r="G9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I9" t="s">
         <v>78</v>
@@ -4606,10 +4631,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M9" t="s">
         <v>116</v>
@@ -4626,13 +4651,13 @@
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E10" s="9">
         <v>615</v>
       </c>
       <c r="G10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>
@@ -4644,10 +4669,10 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M10" t="s">
         <v>116</v>
@@ -4664,13 +4689,13 @@
         <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I11" t="s">
         <v>78</v>
@@ -4679,7 +4704,7 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M11" t="s">
         <v>116</v>
@@ -4693,13 +4718,13 @@
         <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I12" t="s">
         <v>78</v>
@@ -4708,7 +4733,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M12" t="s">
         <v>144</v>
@@ -4722,13 +4747,13 @@
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I13" t="s">
         <v>78</v>
@@ -4737,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M13" t="s">
         <v>144</v>
@@ -4751,13 +4776,13 @@
         <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I14" t="s">
         <v>78</v>
@@ -4766,7 +4791,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="M14" t="s">
         <v>144</v>
@@ -4780,13 +4805,13 @@
         <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I15" t="s">
         <v>78</v>
@@ -4795,7 +4820,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M15" t="s">
         <v>161</v>
@@ -4809,13 +4834,13 @@
         <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I16" t="s">
         <v>78</v>
@@ -4824,7 +4849,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M16" t="s">
         <v>161</v>
@@ -4838,13 +4863,13 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I17" t="s">
         <v>78</v>
@@ -4853,7 +4878,7 @@
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="M17" t="s">
         <v>161</v>
@@ -4867,13 +4892,13 @@
         <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I18" t="s">
         <v>78</v>
@@ -4882,7 +4907,7 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M18" t="s">
         <v>161</v>
@@ -4922,7 +4947,7 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -4934,7 +4959,7 @@
         <v>78</v>
       </c>
       <c r="K20" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="M20" t="s">
         <v>161</v>
@@ -4949,14 +4974,14 @@
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E21" s="13">
         <v>0</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13" t="s">
@@ -4966,7 +4991,7 @@
         <v>1</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L21" s="13"/>
       <c r="M21" s="13" t="s">
@@ -4985,14 +5010,14 @@
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13" t="s">
-        <v>463</v>
+        <v>476</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="13" t="s">
@@ -5000,10 +5025,10 @@
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="13" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="M22" s="13" t="s">
         <v>161</v>
@@ -5013,7 +5038,7 @@
         <v>32350462</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -5155,7 +5180,7 @@
         <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F6" t="s">
         <v>53</v>
@@ -5181,7 +5206,7 @@
         <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F7" t="s">
         <v>53</v>
@@ -5308,10 +5333,10 @@
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F12" t="s">
         <v>92</v>
@@ -5320,7 +5345,7 @@
         <v>94</v>
       </c>
       <c r="I12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K12" t="s">
         <v>116</v>
@@ -5337,7 +5362,7 @@
         <v>97</v>
       </c>
       <c r="E13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F13" t="s">
         <v>92</v>
@@ -5396,11 +5421,11 @@
         <v>92</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="11" t="s">
@@ -5424,10 +5449,10 @@
         <v>92</v>
       </c>
       <c r="G16" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I16" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K16" t="s">
         <v>116</v>
@@ -5519,10 +5544,10 @@
         <v>35</v>
       </c>
       <c r="D20" t="s">
+        <v>238</v>
+      </c>
+      <c r="E20" t="s">
         <v>239</v>
-      </c>
-      <c r="E20" t="s">
-        <v>240</v>
       </c>
       <c r="F20" t="s">
         <v>92</v>
@@ -5531,7 +5556,7 @@
         <v>128</v>
       </c>
       <c r="I20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K20" t="s">
         <v>144</v>
@@ -5548,7 +5573,7 @@
         <v>118</v>
       </c>
       <c r="E21" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F21" t="s">
         <v>92</v>
@@ -5607,11 +5632,11 @@
         <v>92</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J23" s="11"/>
       <c r="K23" s="11" t="s">
@@ -5635,10 +5660,10 @@
         <v>92</v>
       </c>
       <c r="G24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I24" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="K24" t="s">
         <v>144</v>
@@ -5661,10 +5686,10 @@
         <v>92</v>
       </c>
       <c r="G25" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I25" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K25" t="s">
         <v>144</v>
@@ -5705,20 +5730,20 @@
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>92</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J27" s="11"/>
       <c r="K27" s="11" t="s">
@@ -5747,7 +5772,7 @@
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="12" t="s">
@@ -5766,7 +5791,7 @@
         <v>126</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>92</v>
@@ -5776,7 +5801,7 @@
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12" t="s">
@@ -5830,11 +5855,11 @@
         <v>92</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12" t="s">
@@ -5850,20 +5875,20 @@
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12" t="s">
@@ -5882,17 +5907,17 @@
         <v>122</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12" t="s">
@@ -5911,17 +5936,17 @@
         <v>123</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12" t="s">
@@ -5940,17 +5965,17 @@
         <v>124</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>92</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J35" s="11"/>
       <c r="K35" s="11" t="s">
@@ -5969,17 +5994,17 @@
         <v>124</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H36" s="12"/>
       <c r="I36" s="12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J36" s="12"/>
       <c r="K36" s="12" t="s">
@@ -5995,20 +6020,20 @@
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H37" s="12"/>
       <c r="I37" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12" t="s">
@@ -6055,7 +6080,7 @@
         <v>154</v>
       </c>
       <c r="E39" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F39" t="s">
         <v>92</v>
@@ -6079,20 +6104,20 @@
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>92</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J40" s="11"/>
       <c r="K40" s="11" t="s">
@@ -6107,19 +6132,19 @@
         <v>35</v>
       </c>
       <c r="D41" t="s">
+        <v>208</v>
+      </c>
+      <c r="E41" t="s">
         <v>209</v>
-      </c>
-      <c r="E41" t="s">
-        <v>210</v>
       </c>
       <c r="F41" t="s">
         <v>92</v>
       </c>
       <c r="G41" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K41" t="s">
         <v>161</v>
@@ -6137,17 +6162,17 @@
         <v>157</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F42" s="11" t="s">
         <v>92</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H42" s="11"/>
       <c r="I42" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J42" s="11"/>
       <c r="K42" s="11" t="s">
@@ -6165,16 +6190,16 @@
         <v>157</v>
       </c>
       <c r="E43" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F43" t="s">
         <v>92</v>
       </c>
       <c r="G43" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I43" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K43" t="s">
         <v>161</v>
@@ -6197,10 +6222,10 @@
         <v>92</v>
       </c>
       <c r="G44" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I44" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K44" t="s">
         <v>161</v>
@@ -6215,20 +6240,20 @@
       </c>
       <c r="C45" s="13"/>
       <c r="D45" s="13" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>92</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="13" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J45" s="13"/>
       <c r="K45" s="13" t="s">
@@ -6253,7 +6278,7 @@
         <v>92</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H46" s="11"/>
       <c r="I46" s="11" t="s">
@@ -6281,10 +6306,10 @@
         <v>92</v>
       </c>
       <c r="G47" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I47" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K47" t="s">
         <v>161</v>
@@ -6324,19 +6349,19 @@
         <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E49" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F49" t="s">
         <v>92</v>
       </c>
       <c r="G49" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I49" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K49" t="s">
         <v>161</v>

</xml_diff>

<commit_message>
fitting of 3 params of VL sub-model
</commit_message>
<xml_diff>
--- a/src/Cov19_life_cycle/cov19_life_cycle.xlsx
+++ b/src/Cov19_life_cycle/cov19_life_cycle.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80ECC12E-B1DE-42A0-8E2A-2F6F99A58DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Const" sheetId="3" r:id="rId1"/>
@@ -14,9 +15,10 @@
     <sheet name="Reaction" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Const!$H$4:$M$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Reaction!$A$4:$K$49</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="478">
   <si>
     <t>on</t>
   </si>
@@ -1460,12 +1462,15 @@
   </si>
   <si>
     <t xml:space="preserve"> switch_ir*anti_Ab_max*(t/T_sw_ir - 1)^n_ir/((1 + ET50_ir/T_sw_ir)^n_ir + (t/T_sw_ir - 1)^n_ir)</t>
+  </si>
+  <si>
+    <t>doi.org/10.1101/2020.03.05.20030502, 32315724</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1584,7 +1589,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1600,9 +1605,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1640,9 +1645,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1675,9 +1680,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1710,9 +1732,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1885,33 +1924,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomRight" activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="64.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="64.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1943,7 +1982,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1982,7 +2021,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2008,7 +2047,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2034,7 +2073,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>1</v>
       </c>
@@ -2067,7 +2106,7 @@
       </c>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2099,7 +2138,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>0</v>
       </c>
@@ -2134,7 +2173,7 @@
       </c>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2166,7 +2205,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>0</v>
       </c>
@@ -2199,133 +2238,138 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>0</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="15">
         <v>0.25</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" s="11"/>
+      <c r="H12" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="11" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="11">
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="5">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>471</v>
+      </c>
+      <c r="H13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" t="s">
+        <v>373</v>
+      </c>
+      <c r="J13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" t="s">
+        <v>374</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
         <v>0</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E14" s="15">
         <v>0.01</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11" t="s">
+      <c r="G14" s="11"/>
+      <c r="H14" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I14" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J14" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K14" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>0</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E15" s="15">
         <v>0.25</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="H14" t="s">
+      <c r="G15" s="11"/>
+      <c r="H15" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I15" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K15" s="11" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s">
-        <v>234</v>
-      </c>
-      <c r="E15" s="10">
-        <v>1.8</v>
-      </c>
-      <c r="F15" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" t="s">
-        <v>235</v>
-      </c>
-      <c r="I15" t="s">
-        <v>244</v>
-      </c>
-      <c r="J15" t="s">
-        <v>116</v>
-      </c>
-      <c r="K15" t="s">
-        <v>43</v>
-      </c>
-      <c r="L15">
-        <v>20463877</v>
-      </c>
-      <c r="M15" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2333,207 +2377,202 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
+        <v>286</v>
+      </c>
+      <c r="E16" s="5">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>471</v>
+      </c>
+      <c r="H16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" t="s">
+        <v>373</v>
+      </c>
+      <c r="J16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" t="s">
+        <v>374</v>
+      </c>
+      <c r="L16" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>234</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" t="s">
+        <v>235</v>
+      </c>
+      <c r="I17" t="s">
+        <v>244</v>
+      </c>
+      <c r="J17" t="s">
+        <v>116</v>
+      </c>
+      <c r="K17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17">
+        <v>20463877</v>
+      </c>
+      <c r="M17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
         <v>182</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E18" s="6">
         <v>23.56</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F18" t="s">
         <v>67</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H18" t="s">
         <v>186</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I18" t="s">
         <v>221</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J18" t="s">
         <v>116</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K18" t="s">
         <v>43</v>
       </c>
-      <c r="L16">
+      <c r="L18">
         <v>32225176</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M18" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="13">
-        <v>1</v>
-      </c>
-      <c r="B17" s="13" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="13">
+        <v>1</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E19" s="6">
         <v>150</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F19" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13" t="s">
+      <c r="G19" s="13"/>
+      <c r="H19" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I19" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13" t="s">
+      <c r="J19" s="13"/>
+      <c r="K19" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="11">
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="11">
         <v>0</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E20" s="15">
         <v>31.13</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11" t="s">
+      <c r="G20" s="11"/>
+      <c r="H20" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11" t="s">
+      <c r="I20" s="11"/>
+      <c r="J20" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L20" s="11">
         <v>32225176</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M20" s="11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
         <v>36</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>451</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E21" s="6">
         <v>4670</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>145</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H21" t="s">
         <v>452</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I21" t="s">
         <v>453</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J21" t="s">
         <v>116</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K21" t="s">
         <v>43</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <v>32225176</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M21" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>189</v>
-      </c>
-      <c r="E20" s="8">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="F20" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" t="s">
-        <v>190</v>
-      </c>
-      <c r="I20" t="s">
-        <v>224</v>
-      </c>
-      <c r="J20" t="s">
-        <v>144</v>
-      </c>
-      <c r="K20" t="s">
-        <v>90</v>
-      </c>
-      <c r="L20">
-        <v>9894006</v>
-      </c>
-      <c r="M20" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="11">
-        <v>0</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11" t="s">
-        <v>411</v>
-      </c>
-      <c r="E21" s="8">
-        <v>1</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L21" s="11">
-        <v>15384040</v>
-      </c>
-      <c r="M21" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2541,106 +2580,106 @@
         <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>411</v>
+        <v>189</v>
       </c>
       <c r="E22" s="8">
-        <v>2</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="F22" t="s">
         <v>67</v>
       </c>
       <c r="H22" t="s">
+        <v>190</v>
+      </c>
+      <c r="I22" t="s">
+        <v>224</v>
+      </c>
+      <c r="J22" t="s">
+        <v>144</v>
+      </c>
+      <c r="K22" t="s">
+        <v>90</v>
+      </c>
+      <c r="L22">
+        <v>9894006</v>
+      </c>
+      <c r="M22" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
+        <v>0</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I23" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L23" s="11">
+        <v>15384040</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>411</v>
+      </c>
+      <c r="E24" s="8">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" t="s">
+        <v>206</v>
+      </c>
+      <c r="I24" t="s">
         <v>377</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J24" t="s">
         <v>161</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K24" t="s">
         <v>374</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L24" t="s">
         <v>375</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M24" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s">
-        <v>193</v>
-      </c>
-      <c r="E23" s="8">
-        <v>14</v>
-      </c>
-      <c r="F23" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" t="s">
-        <v>197</v>
-      </c>
-      <c r="I23" t="s">
-        <v>226</v>
-      </c>
-      <c r="J23" t="s">
-        <v>161</v>
-      </c>
-      <c r="K23" t="s">
-        <v>43</v>
-      </c>
-      <c r="L23">
-        <v>15384040</v>
-      </c>
-      <c r="M23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="11">
-        <v>0</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="E24" s="10">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="L24" s="11">
-        <v>15384040</v>
-      </c>
-      <c r="M24" s="11" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2648,69 +2687,71 @@
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>194</v>
-      </c>
-      <c r="E25" s="10">
-        <v>0.5</v>
+        <v>193</v>
+      </c>
+      <c r="E25" s="8">
+        <v>14</v>
       </c>
       <c r="F25" t="s">
         <v>67</v>
       </c>
       <c r="H25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I25" t="s">
-        <v>377</v>
+        <v>226</v>
       </c>
       <c r="J25" t="s">
         <v>161</v>
       </c>
       <c r="K25" t="s">
-        <v>374</v>
-      </c>
-      <c r="L25" t="s">
-        <v>375</v>
+        <v>43</v>
+      </c>
+      <c r="L25">
+        <v>15384040</v>
       </c>
       <c r="M25" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="11">
+        <v>0</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D26" t="s">
-        <v>195</v>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="E26" s="10">
-        <v>9992</v>
-      </c>
-      <c r="F26" t="s">
-        <v>145</v>
-      </c>
-      <c r="H26" t="s">
-        <v>199</v>
-      </c>
-      <c r="I26" t="s">
-        <v>405</v>
-      </c>
-      <c r="J26" t="s">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="J26" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="11">
         <v>15384040</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>0</v>
       </c>
@@ -2719,35 +2760,35 @@
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="E27" s="10">
-        <v>0.14000000000000001</v>
+        <v>194</v>
+      </c>
+      <c r="E27" s="15">
+        <v>0.5</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>67</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>232</v>
+        <v>377</v>
       </c>
       <c r="J27" s="11" t="s">
         <v>161</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="L27" s="11">
-        <v>15384040</v>
+        <v>374</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>375</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2755,16 +2796,16 @@
         <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="E28" s="10">
-        <v>0.39</v>
+        <v>0.2</v>
       </c>
       <c r="F28" t="s">
         <v>67</v>
       </c>
       <c r="H28" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="I28" t="s">
         <v>377</v>
@@ -2773,7 +2814,7 @@
         <v>161</v>
       </c>
       <c r="K28" t="s">
-        <v>229</v>
+        <v>374</v>
       </c>
       <c r="L28" t="s">
         <v>375</v>
@@ -2782,7 +2823,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2790,69 +2831,71 @@
         <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>196</v>
-      </c>
-      <c r="E29" s="6">
-        <v>0.17</v>
+        <v>195</v>
+      </c>
+      <c r="E29" s="10">
+        <v>9992</v>
       </c>
       <c r="F29" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="H29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I29" t="s">
-        <v>223</v>
+        <v>405</v>
       </c>
       <c r="J29" t="s">
         <v>161</v>
       </c>
       <c r="K29" t="s">
-        <v>90</v>
+        <v>229</v>
       </c>
       <c r="L29">
-        <v>32182409</v>
+        <v>15384040</v>
       </c>
       <c r="M29" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="11">
+        <v>0</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D30" t="s">
-        <v>378</v>
-      </c>
-      <c r="E30" s="6">
-        <v>11900</v>
-      </c>
-      <c r="F30" t="s">
-        <v>256</v>
-      </c>
-      <c r="H30" t="s">
-        <v>379</v>
-      </c>
-      <c r="I30" t="s">
-        <v>380</v>
-      </c>
-      <c r="J30" t="s">
-        <v>116</v>
-      </c>
-      <c r="K30" t="s">
-        <v>90</v>
-      </c>
-      <c r="L30">
-        <v>7103258</v>
-      </c>
-      <c r="M30" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C30" s="11"/>
+      <c r="D30" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E30" s="10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="L30" s="11">
+        <v>15384040</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2860,127 +2903,133 @@
         <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>394</v>
-      </c>
-      <c r="E31" s="6">
-        <v>17</v>
+        <v>212</v>
+      </c>
+      <c r="E31" s="10">
+        <v>0.39</v>
       </c>
       <c r="F31" t="s">
         <v>67</v>
       </c>
       <c r="H31" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="I31" t="s">
-        <v>396</v>
+        <v>377</v>
       </c>
       <c r="J31" t="s">
         <v>161</v>
       </c>
       <c r="K31" t="s">
+        <v>229</v>
+      </c>
+      <c r="L31" t="s">
+        <v>375</v>
+      </c>
+      <c r="M31" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" t="s">
+        <v>200</v>
+      </c>
+      <c r="I32" t="s">
+        <v>223</v>
+      </c>
+      <c r="J32" t="s">
+        <v>161</v>
+      </c>
+      <c r="K32" t="s">
+        <v>90</v>
+      </c>
+      <c r="L32">
+        <v>32182409</v>
+      </c>
+      <c r="M32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="s">
+        <v>378</v>
+      </c>
+      <c r="E33" s="6">
+        <v>11900</v>
+      </c>
+      <c r="F33" t="s">
+        <v>256</v>
+      </c>
+      <c r="H33" t="s">
+        <v>379</v>
+      </c>
+      <c r="I33" t="s">
+        <v>380</v>
+      </c>
+      <c r="J33" t="s">
+        <v>116</v>
+      </c>
+      <c r="K33" t="s">
+        <v>90</v>
+      </c>
+      <c r="L33">
+        <v>7103258</v>
+      </c>
+      <c r="M33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" t="s">
+        <v>394</v>
+      </c>
+      <c r="E34" s="6">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" t="s">
+        <v>395</v>
+      </c>
+      <c r="I34" t="s">
+        <v>396</v>
+      </c>
+      <c r="J34" t="s">
+        <v>161</v>
+      </c>
+      <c r="K34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="13">
-        <v>1</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="E32" s="14">
-        <v>0</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13" t="s">
-        <v>434</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>435</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A33" s="13">
-        <v>1</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13" t="s">
-        <v>431</v>
-      </c>
-      <c r="E33" s="13">
-        <v>50</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>439</v>
-      </c>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J33" s="13" t="s">
-        <v>435</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A34" s="13">
-        <v>1</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13" t="s">
-        <v>437</v>
-      </c>
-      <c r="E34" s="14">
-        <v>190</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>439</v>
-      </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13" t="s">
-        <v>438</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>435</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>1</v>
       </c>
@@ -2989,17 +3038,17 @@
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E35" s="14">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="F35" s="13" t="s">
         <v>89</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="I35" s="13" t="s">
         <v>42</v>
@@ -3013,7 +3062,7 @@
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>1</v>
       </c>
@@ -3022,17 +3071,17 @@
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="E36" s="14">
-        <v>5</v>
+        <v>431</v>
+      </c>
+      <c r="E36" s="13">
+        <v>50</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>89</v>
+        <v>439</v>
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="13" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I36" s="13" t="s">
         <v>42</v>
@@ -3046,7 +3095,7 @@
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>1</v>
       </c>
@@ -3055,33 +3104,31 @@
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="E37" s="14">
-        <v>14300</v>
+        <v>190</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>145</v>
+        <v>439</v>
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>458</v>
+        <v>42</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>161</v>
+        <v>435</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="L37" s="13">
-        <v>32404477</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="L37" s="13"/>
       <c r="M37" s="13"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>1</v>
       </c>
@@ -3090,20 +3137,20 @@
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13" t="s">
-        <v>461</v>
+        <v>432</v>
       </c>
       <c r="E38" s="14">
-        <v>941000</v>
+        <v>700</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="13" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>462</v>
+        <v>42</v>
       </c>
       <c r="J38" s="13" t="s">
         <v>435</v>
@@ -3111,104 +3158,206 @@
       <c r="K38" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="L38" s="13">
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" s="13">
+        <v>1</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="E39" s="14">
+        <v>5</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="K39" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="13">
+        <v>1</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="E40" s="14">
+        <v>14300</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="K40" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L40" s="13">
+        <v>32404477</v>
+      </c>
+      <c r="M40" s="13"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="13">
+        <v>1</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="E41" s="14">
+        <v>941000</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="J41" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L41" s="13">
         <v>15358653</v>
       </c>
-      <c r="M38" s="13"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A39" s="12">
-        <v>1</v>
-      </c>
-      <c r="B39" s="12" t="s">
+      <c r="M41" s="13"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="12">
+        <v>1</v>
+      </c>
+      <c r="B42" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12" t="s">
+      <c r="C42" s="12"/>
+      <c r="D42" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E42" s="12">
         <v>1.33E-12</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F42" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12" t="s">
+      <c r="G42" s="12"/>
+      <c r="H42" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I39" s="12" t="s">
+      <c r="I42" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12" t="s">
+      <c r="J42" s="12"/>
+      <c r="K42" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="L39" s="12">
+      <c r="L42" s="12">
         <v>7103258</v>
       </c>
-      <c r="M39" s="12" t="s">
+      <c r="M42" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
-      <c r="P39" s="12"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A40" s="12">
-        <v>1</v>
-      </c>
-      <c r="B40" s="12" t="s">
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="12"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="12">
+        <v>1</v>
+      </c>
+      <c r="B43" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12" t="s">
+      <c r="C43" s="12"/>
+      <c r="D43" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E43" s="16">
         <v>1000</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F43" s="12" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="62" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H62">
+    <row r="65" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H65">
         <v>44</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="H4:M42" xr:uid="{B71E45CA-F913-46E1-9314-D29A180B8B1F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="6.453125" customWidth="1"/>
-    <col min="4" max="4" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="70.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" customWidth="1"/>
-    <col min="9" max="9" width="17.90625" customWidth="1"/>
-    <col min="10" max="10" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="70.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3243,7 +3392,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -3278,7 +3427,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3302,7 +3451,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3326,7 +3475,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3349,7 +3498,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3372,7 +3521,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>1</v>
       </c>
@@ -3399,7 +3548,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>1</v>
       </c>
@@ -3428,7 +3577,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3451,7 +3600,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3474,7 +3623,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3497,7 +3646,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3520,7 +3669,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -3543,7 +3692,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -3566,7 +3715,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3589,7 +3738,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3612,7 +3761,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>1</v>
       </c>
@@ -3639,7 +3788,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -3662,7 +3811,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>0</v>
       </c>
@@ -3689,7 +3838,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3712,7 +3861,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3735,7 +3884,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -3758,7 +3907,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -3781,7 +3930,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -3804,7 +3953,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
@@ -3827,7 +3976,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -3850,7 +3999,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -3873,7 +4022,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
@@ -3896,7 +4045,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -3919,7 +4068,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -3942,7 +4091,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
@@ -3965,7 +4114,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
@@ -3988,7 +4137,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
@@ -4011,7 +4160,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <v>0</v>
       </c>
@@ -4038,7 +4187,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
@@ -4061,7 +4210,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>1</v>
       </c>
@@ -4088,7 +4237,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>1</v>
       </c>
@@ -4121,32 +4270,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.08984375" customWidth="1"/>
-    <col min="11" max="11" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.109375" customWidth="1"/>
+    <col min="11" max="11" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4181,7 +4330,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -4225,7 +4374,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>0</v>
       </c>
@@ -4253,7 +4402,7 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4285,7 +4434,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>0</v>
       </c>
@@ -4317,7 +4466,7 @@
       </c>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>0</v>
       </c>
@@ -4359,34 +4508,34 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="74" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4427,7 +4576,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -4477,7 +4626,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4515,7 +4664,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4541,7 +4690,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4567,7 +4716,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -4608,7 +4757,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -4643,7 +4792,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -4681,7 +4830,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4710,7 +4859,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4739,7 +4888,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4768,7 +4917,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -4797,7 +4946,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -4826,7 +4975,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -4855,7 +5004,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -4884,7 +5033,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -4913,7 +5062,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -4924,7 +5073,7 @@
         <v>75</v>
       </c>
       <c r="E19" s="5">
-        <v>4.0000000000000002E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="G19" t="s">
         <v>145</v>
@@ -4939,7 +5088,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -4965,7 +5114,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>1</v>
       </c>
@@ -5001,7 +5150,7 @@
       <c r="O21" s="13"/>
       <c r="P21" s="13"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>1</v>
       </c>
@@ -5048,32 +5197,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.36328125" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5108,7 +5257,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -5143,7 +5292,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5169,7 +5318,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5195,7 +5344,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -5221,7 +5370,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -5247,7 +5396,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -5273,7 +5422,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -5299,7 +5448,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -5325,7 +5474,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -5351,7 +5500,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -5377,7 +5526,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -5403,7 +5552,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>0</v>
       </c>
@@ -5432,7 +5581,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -5458,7 +5607,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -5484,7 +5633,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -5510,7 +5659,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -5536,7 +5685,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -5562,7 +5711,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5588,7 +5737,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -5614,7 +5763,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>0</v>
       </c>
@@ -5643,7 +5792,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -5669,7 +5818,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -5695,7 +5844,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -5721,7 +5870,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>0</v>
       </c>
@@ -5750,7 +5899,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>1</v>
       </c>
@@ -5779,7 +5928,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>1</v>
       </c>
@@ -5808,7 +5957,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>1</v>
       </c>
@@ -5837,7 +5986,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>1</v>
       </c>
@@ -5866,7 +6015,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -5895,7 +6044,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>1</v>
       </c>
@@ -5924,7 +6073,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>1</v>
       </c>
@@ -5953,7 +6102,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <v>0</v>
       </c>
@@ -5982,7 +6131,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -6011,7 +6160,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>1</v>
       </c>
@@ -6040,7 +6189,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>1</v>
       </c>
@@ -6069,7 +6218,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1</v>
       </c>
@@ -6095,7 +6244,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>0</v>
       </c>
@@ -6124,7 +6273,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1</v>
       </c>
@@ -6150,7 +6299,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>0</v>
       </c>
@@ -6179,7 +6328,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1</v>
       </c>
@@ -6205,7 +6354,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1</v>
       </c>
@@ -6231,7 +6380,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>1</v>
       </c>
@@ -6260,7 +6409,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
         <v>0</v>
       </c>
@@ -6289,7 +6438,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1</v>
       </c>
@@ -6315,7 +6464,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1</v>
       </c>
@@ -6341,7 +6490,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1</v>
       </c>
@@ -6368,7 +6517,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:K49"/>
+  <autoFilter ref="A4:K49" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
kbase_tran_ units corrected to 1/pM/h
</commit_message>
<xml_diff>
--- a/src/Cov19_life_cycle/cov19_life_cycle.xlsx
+++ b/src/Cov19_life_cycle/cov19_life_cycle.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21033B6-D884-492B-A125-4C12EB0505D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Const" sheetId="3" r:id="rId1"/>
@@ -18,19 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Reaction!$A$4:$K$49</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="479">
   <si>
     <t>on</t>
   </si>
@@ -1464,12 +1457,15 @@
   </si>
   <si>
     <t>doi.org/10.1101/2020.03.05.20030502, 32315724</t>
+  </si>
+  <si>
+    <t>1/pM/h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1588,7 +1584,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1604,9 +1600,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1644,9 +1640,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1679,9 +1675,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1714,9 +1727,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1889,33 +1919,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K35" sqref="A35:K35"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="64.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="64.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1947,7 +1977,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1986,7 +2016,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2012,7 +2042,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2038,7 +2068,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>1</v>
       </c>
@@ -2071,7 +2101,7 @@
       </c>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2103,7 +2133,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>0</v>
       </c>
@@ -2138,7 +2168,7 @@
       </c>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2170,7 +2200,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>0</v>
       </c>
@@ -2203,7 +2233,7 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>0</v>
       </c>
@@ -2236,7 +2266,7 @@
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2250,7 +2280,7 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="H13" t="s">
         <v>72</v>
@@ -2268,7 +2298,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>0</v>
       </c>
@@ -2301,7 +2331,7 @@
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>0</v>
       </c>
@@ -2334,7 +2364,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2348,7 +2378,7 @@
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="H16" t="s">
         <v>73</v>
@@ -2366,7 +2396,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2401,7 +2431,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2436,7 +2466,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>1</v>
       </c>
@@ -2467,7 +2497,7 @@
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>0</v>
       </c>
@@ -2502,7 +2532,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2537,7 +2567,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2572,7 +2602,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>0</v>
       </c>
@@ -2609,7 +2639,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2644,7 +2674,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2679,7 +2709,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>0</v>
       </c>
@@ -2716,7 +2746,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>0</v>
       </c>
@@ -2753,7 +2783,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2788,7 +2818,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2823,7 +2853,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>0</v>
       </c>
@@ -2860,7 +2890,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2895,7 +2925,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2930,7 +2960,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2965,7 +2995,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2994,7 +3024,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>0</v>
       </c>
@@ -3027,7 +3057,7 @@
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>1</v>
       </c>
@@ -3060,7 +3090,7 @@
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>1</v>
       </c>
@@ -3093,7 +3123,7 @@
       <c r="L37" s="13"/>
       <c r="M37" s="13"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>1</v>
       </c>
@@ -3126,7 +3156,7 @@
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>1</v>
       </c>
@@ -3159,7 +3189,7 @@
       <c r="L39" s="13"/>
       <c r="M39" s="13"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>1</v>
       </c>
@@ -3194,7 +3224,7 @@
       </c>
       <c r="M40" s="13"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>1</v>
       </c>
@@ -3229,7 +3259,7 @@
       </c>
       <c r="M41" s="13"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>1</v>
       </c>
@@ -3267,7 +3297,7 @@
       <c r="O42" s="12"/>
       <c r="P42" s="12"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>1</v>
       </c>
@@ -3285,44 +3315,44 @@
         <v>473</v>
       </c>
     </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H65">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H4:M42"/>
+  <autoFilter ref="H4:M42" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="6.453125" customWidth="1"/>
-    <col min="4" max="4" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="70.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" customWidth="1"/>
-    <col min="9" max="9" width="17.90625" customWidth="1"/>
-    <col min="10" max="10" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="70.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3357,7 +3387,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -3392,7 +3422,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3416,7 +3446,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3440,7 +3470,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3463,7 +3493,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3486,7 +3516,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>1</v>
       </c>
@@ -3513,7 +3543,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>1</v>
       </c>
@@ -3542,7 +3572,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3565,7 +3595,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3588,7 +3618,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3611,7 +3641,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3634,7 +3664,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -3657,7 +3687,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -3680,7 +3710,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3703,7 +3733,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3726,7 +3756,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>1</v>
       </c>
@@ -3753,7 +3783,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -3776,7 +3806,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>0</v>
       </c>
@@ -3803,7 +3833,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3826,7 +3856,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3849,7 +3879,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -3872,7 +3902,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -3895,7 +3925,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -3918,7 +3948,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
@@ -3941,7 +3971,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -3964,7 +3994,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -3987,7 +4017,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
@@ -4010,7 +4040,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -4033,7 +4063,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -4056,7 +4086,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
@@ -4079,7 +4109,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
@@ -4102,7 +4132,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
@@ -4125,7 +4155,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <v>0</v>
       </c>
@@ -4152,7 +4182,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
@@ -4175,7 +4205,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>1</v>
       </c>
@@ -4202,7 +4232,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>1</v>
       </c>
@@ -4229,7 +4259,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1</v>
       </c>
@@ -4261,32 +4291,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.08984375" customWidth="1"/>
-    <col min="11" max="11" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.109375" customWidth="1"/>
+    <col min="11" max="11" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4321,7 +4351,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -4365,7 +4395,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>0</v>
       </c>
@@ -4393,7 +4423,7 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4425,7 +4455,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>0</v>
       </c>
@@ -4457,7 +4487,7 @@
       </c>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>0</v>
       </c>
@@ -4499,34 +4529,34 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="74" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4567,7 +4597,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -4617,7 +4647,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4655,7 +4685,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4681,7 +4711,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4707,7 +4737,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -4748,7 +4778,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -4783,7 +4813,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -4821,7 +4851,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4850,7 +4880,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4879,7 +4909,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4908,7 +4938,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -4937,7 +4967,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -4966,7 +4996,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -4995,7 +5025,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -5024,7 +5054,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -5053,7 +5083,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -5079,7 +5109,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -5105,7 +5135,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>1</v>
       </c>
@@ -5141,7 +5171,7 @@
       <c r="O21" s="13"/>
       <c r="P21" s="13"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>1</v>
       </c>
@@ -5188,7 +5218,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5198,22 +5228,22 @@
       <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.36328125" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5248,7 +5278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -5283,7 +5313,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5309,7 +5339,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5335,7 +5365,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -5361,7 +5391,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -5387,7 +5417,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -5413,7 +5443,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -5439,7 +5469,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -5465,7 +5495,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -5491,7 +5521,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -5517,7 +5547,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -5543,7 +5573,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>0</v>
       </c>
@@ -5572,7 +5602,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -5598,7 +5628,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -5624,7 +5654,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -5650,7 +5680,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -5676,7 +5706,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -5702,7 +5732,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5728,7 +5758,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -5754,7 +5784,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>0</v>
       </c>
@@ -5783,7 +5813,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -5809,7 +5839,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -5835,7 +5865,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -5861,7 +5891,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>0</v>
       </c>
@@ -5890,7 +5920,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>1</v>
       </c>
@@ -5919,7 +5949,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>1</v>
       </c>
@@ -5948,7 +5978,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>1</v>
       </c>
@@ -5977,7 +6007,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>1</v>
       </c>
@@ -6006,7 +6036,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -6035,7 +6065,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>1</v>
       </c>
@@ -6064,7 +6094,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>1</v>
       </c>
@@ -6093,7 +6123,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <v>0</v>
       </c>
@@ -6122,7 +6152,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -6151,7 +6181,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>1</v>
       </c>
@@ -6180,7 +6210,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>1</v>
       </c>
@@ -6209,7 +6239,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1</v>
       </c>
@@ -6235,7 +6265,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>0</v>
       </c>
@@ -6264,7 +6294,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1</v>
       </c>
@@ -6290,7 +6320,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>0</v>
       </c>
@@ -6319,7 +6349,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1</v>
       </c>
@@ -6345,7 +6375,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1</v>
       </c>
@@ -6371,7 +6401,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>1</v>
       </c>
@@ -6400,7 +6430,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
         <v>0</v>
       </c>
@@ -6429,7 +6459,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1</v>
       </c>
@@ -6455,7 +6485,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1</v>
       </c>
@@ -6481,7 +6511,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1</v>
       </c>
@@ -6508,7 +6538,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:K49"/>
+  <autoFilter ref="A4:K49" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
error correction in V_tran_ and k_tran_
</commit_message>
<xml_diff>
--- a/src/Cov19_life_cycle/cov19_life_cycle.xlsx
+++ b/src/Cov19_life_cycle/cov19_life_cycle.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21033B6-D884-492B-A125-4C12EB0505D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A76928C-F09D-47C9-9D1C-6C5BA2B0F040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,15 +15,15 @@
     <sheet name="Reaction" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Const!$H$4:$M$42</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Reaction!$A$4:$K$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Const!$H$4:$M$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Reaction!$A$4:$K$51</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="483">
   <si>
     <t>on</t>
   </si>
@@ -1460,6 +1460,18 @@
   </si>
   <si>
     <t>1/pM/h</t>
+  </si>
+  <si>
+    <t>Vol_alv*k_tran_pc_ipc*PC</t>
+  </si>
+  <si>
+    <t>Vol_alv*k_tran_ipc_vpc*iPC</t>
+  </si>
+  <si>
+    <t>kbase_tran_pc_ipc*COV_ACE2_pc/Vol_alv</t>
+  </si>
+  <si>
+    <t>kbase_tran_ipc_vpc*COV_ipc/Vol_alv</t>
   </si>
 </sst>
 </file>
@@ -1920,13 +1932,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2267,69 +2279,71 @@
       <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="11">
+        <v>0</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="15">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" s="5">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
         <v>478</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>72</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I14" t="s">
         <v>373</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J14" t="s">
         <v>65</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K14" t="s">
         <v>374</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L14" s="12" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
-        <v>0</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="E14" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>471</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
@@ -2343,7 +2357,7 @@
         <v>286</v>
       </c>
       <c r="E15" s="15">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>471</v>
@@ -2359,77 +2373,78 @@
         <v>65</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>374</v>
+        <v>42</v>
       </c>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="11">
+        <v>0</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
+        <v>0</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="E17" s="15">
         <v>10</v>
       </c>
-      <c r="F16" t="s">
-        <v>478</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="F17" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J17" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K17" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L17" s="11" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>234</v>
-      </c>
-      <c r="E17" s="10">
-        <v>1.8</v>
-      </c>
-      <c r="F17" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" t="s">
-        <v>235</v>
-      </c>
-      <c r="I17" t="s">
-        <v>244</v>
-      </c>
-      <c r="J17" t="s">
-        <v>116</v>
-      </c>
-      <c r="K17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17">
-        <v>20463877</v>
-      </c>
-      <c r="M17" t="s">
-        <v>233</v>
-      </c>
+      <c r="M17" s="11"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -2439,204 +2454,199 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
+        <v>286</v>
+      </c>
+      <c r="E18" s="5">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>478</v>
+      </c>
+      <c r="H18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" t="s">
+        <v>373</v>
+      </c>
+      <c r="J18" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" t="s">
+        <v>374</v>
+      </c>
+      <c r="L18" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>234</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" t="s">
+        <v>235</v>
+      </c>
+      <c r="I19" t="s">
+        <v>244</v>
+      </c>
+      <c r="J19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19">
+        <v>20463877</v>
+      </c>
+      <c r="M19" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
         <v>182</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E20" s="6">
         <v>23.56</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F20" t="s">
         <v>67</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H20" t="s">
         <v>186</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I20" t="s">
         <v>221</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J20" t="s">
         <v>116</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K20" t="s">
         <v>43</v>
       </c>
-      <c r="L18">
+      <c r="L20">
         <v>32225176</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M20" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="13">
-        <v>1</v>
-      </c>
-      <c r="B19" s="13" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="13">
+        <v>1</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13" t="s">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E21" s="6">
         <v>150</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F21" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13" t="s">
+      <c r="G21" s="13"/>
+      <c r="H21" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I21" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13" t="s">
+      <c r="J21" s="13"/>
+      <c r="K21" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="11">
         <v>0</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E22" s="15">
         <v>31.13</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11" t="s">
+      <c r="G22" s="11"/>
+      <c r="H22" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11" t="s">
+      <c r="I22" s="11"/>
+      <c r="J22" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K22" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L22" s="11">
         <v>32225176</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M22" s="11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>451</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E23" s="6">
         <v>4670</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F23" t="s">
         <v>145</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H23" t="s">
         <v>452</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I23" t="s">
         <v>453</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J23" t="s">
         <v>116</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K23" t="s">
         <v>43</v>
       </c>
-      <c r="L21">
+      <c r="L23">
         <v>32225176</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M23" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" t="s">
-        <v>189</v>
-      </c>
-      <c r="E22" s="8">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="F22" t="s">
-        <v>67</v>
-      </c>
-      <c r="H22" t="s">
-        <v>190</v>
-      </c>
-      <c r="I22" t="s">
-        <v>224</v>
-      </c>
-      <c r="J22" t="s">
-        <v>144</v>
-      </c>
-      <c r="K22" t="s">
-        <v>90</v>
-      </c>
-      <c r="L22">
-        <v>9894006</v>
-      </c>
-      <c r="M22" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="11">
-        <v>0</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11" t="s">
-        <v>411</v>
-      </c>
-      <c r="E23" s="8">
-        <v>1</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L23" s="11">
-        <v>15384040</v>
-      </c>
-      <c r="M23" s="11" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -2647,247 +2657,247 @@
         <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>411</v>
+        <v>189</v>
       </c>
       <c r="E24" s="8">
-        <v>2</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="F24" t="s">
         <v>67</v>
       </c>
       <c r="H24" t="s">
+        <v>190</v>
+      </c>
+      <c r="I24" t="s">
+        <v>224</v>
+      </c>
+      <c r="J24" t="s">
+        <v>144</v>
+      </c>
+      <c r="K24" t="s">
+        <v>90</v>
+      </c>
+      <c r="L24">
+        <v>9894006</v>
+      </c>
+      <c r="M24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="11">
+        <v>0</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="E25" s="8">
+        <v>1</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I25" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L25" s="11">
+        <v>15384040</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>411</v>
+      </c>
+      <c r="E26" s="8">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" t="s">
+        <v>206</v>
+      </c>
+      <c r="I26" t="s">
         <v>377</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J26" t="s">
         <v>161</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K26" t="s">
         <v>374</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L26" t="s">
         <v>375</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M26" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
         <v>36</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D27" t="s">
         <v>193</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E27" s="8">
         <v>14</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F27" t="s">
         <v>67</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H27" t="s">
         <v>197</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I27" t="s">
         <v>226</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J27" t="s">
         <v>161</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K27" t="s">
         <v>43</v>
       </c>
-      <c r="L25">
+      <c r="L27">
         <v>15384040</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M27" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="11">
         <v>0</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11" t="s">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E28" s="10">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11" t="s">
+      <c r="G28" s="11"/>
+      <c r="H28" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="I28" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="J28" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="K28" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L28" s="11">
         <v>15384040</v>
       </c>
-      <c r="M26" s="11" t="s">
+      <c r="M28" s="11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="11">
         <v>0</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E29" s="15">
         <v>0.5</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11" t="s">
+      <c r="G29" s="11"/>
+      <c r="H29" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I29" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J29" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="K27" s="11" t="s">
+      <c r="K29" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="L27" s="11" t="s">
+      <c r="L29" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="M27" s="11" t="s">
+      <c r="M29" s="11" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
         <v>36</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D30" t="s">
         <v>194</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E30" s="10">
         <v>0.2</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F30" t="s">
         <v>67</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H30" t="s">
         <v>198</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I30" t="s">
         <v>377</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J30" t="s">
         <v>161</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K30" t="s">
         <v>374</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L30" t="s">
         <v>375</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M30" t="s">
         <v>376</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" t="s">
-        <v>195</v>
-      </c>
-      <c r="E29" s="10">
-        <v>9992</v>
-      </c>
-      <c r="F29" t="s">
-        <v>145</v>
-      </c>
-      <c r="H29" t="s">
-        <v>199</v>
-      </c>
-      <c r="I29" t="s">
-        <v>405</v>
-      </c>
-      <c r="J29" t="s">
-        <v>161</v>
-      </c>
-      <c r="K29" t="s">
-        <v>229</v>
-      </c>
-      <c r="L29">
-        <v>15384040</v>
-      </c>
-      <c r="M29" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="11">
-        <v>0</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="E30" s="10">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="L30" s="11">
-        <v>15384040</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -2898,19 +2908,19 @@
         <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="E31" s="10">
-        <v>0.39</v>
+        <v>9992</v>
       </c>
       <c r="F31" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="H31" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="I31" t="s">
-        <v>377</v>
+        <v>405</v>
       </c>
       <c r="J31" t="s">
         <v>161</v>
@@ -2918,46 +2928,48 @@
       <c r="K31" t="s">
         <v>229</v>
       </c>
-      <c r="L31" t="s">
-        <v>375</v>
+      <c r="L31">
+        <v>15384040</v>
       </c>
       <c r="M31" t="s">
-        <v>376</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="A32" s="11">
+        <v>0</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D32" t="s">
-        <v>196</v>
-      </c>
-      <c r="E32" s="6">
-        <v>0.17</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="C32" s="11"/>
+      <c r="D32" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E32" s="10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="H32" t="s">
-        <v>200</v>
-      </c>
-      <c r="I32" t="s">
-        <v>223</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="G32" s="11"/>
+      <c r="H32" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="J32" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="K32" t="s">
-        <v>90</v>
-      </c>
-      <c r="L32">
-        <v>32182409</v>
-      </c>
-      <c r="M32" t="s">
-        <v>222</v>
+      <c r="K32" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="L32" s="11">
+        <v>15384040</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
@@ -2968,31 +2980,31 @@
         <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>378</v>
-      </c>
-      <c r="E33" s="6">
-        <v>11900</v>
+        <v>212</v>
+      </c>
+      <c r="E33" s="10">
+        <v>0.39</v>
       </c>
       <c r="F33" t="s">
-        <v>256</v>
+        <v>67</v>
       </c>
       <c r="H33" t="s">
-        <v>379</v>
+        <v>213</v>
       </c>
       <c r="I33" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="J33" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="K33" t="s">
-        <v>90</v>
-      </c>
-      <c r="L33">
-        <v>7103258</v>
+        <v>229</v>
+      </c>
+      <c r="L33" t="s">
+        <v>375</v>
       </c>
       <c r="M33" t="s">
-        <v>214</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
@@ -3003,113 +3015,117 @@
         <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>394</v>
+        <v>196</v>
       </c>
       <c r="E34" s="6">
-        <v>17</v>
+        <v>0.17</v>
       </c>
       <c r="F34" t="s">
         <v>67</v>
       </c>
       <c r="H34" t="s">
-        <v>395</v>
+        <v>200</v>
       </c>
       <c r="I34" t="s">
-        <v>396</v>
+        <v>223</v>
       </c>
       <c r="J34" t="s">
         <v>161</v>
       </c>
       <c r="K34" t="s">
+        <v>90</v>
+      </c>
+      <c r="L34">
+        <v>32182409</v>
+      </c>
+      <c r="M34" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>378</v>
+      </c>
+      <c r="E35" s="6">
+        <v>11900</v>
+      </c>
+      <c r="F35" t="s">
+        <v>256</v>
+      </c>
+      <c r="H35" t="s">
+        <v>379</v>
+      </c>
+      <c r="I35" t="s">
+        <v>380</v>
+      </c>
+      <c r="J35" t="s">
+        <v>116</v>
+      </c>
+      <c r="K35" t="s">
+        <v>90</v>
+      </c>
+      <c r="L35">
+        <v>7103258</v>
+      </c>
+      <c r="M35" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" t="s">
+        <v>394</v>
+      </c>
+      <c r="E36" s="6">
+        <v>17</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" t="s">
+        <v>395</v>
+      </c>
+      <c r="I36" t="s">
+        <v>396</v>
+      </c>
+      <c r="J36" t="s">
+        <v>161</v>
+      </c>
+      <c r="K36" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="13">
-        <v>0</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="E35" s="14">
-        <v>0</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13" t="s">
-        <v>434</v>
-      </c>
-      <c r="I35" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J35" s="13" t="s">
-        <v>435</v>
-      </c>
-      <c r="K35" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="13">
-        <v>1</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13" t="s">
-        <v>431</v>
-      </c>
-      <c r="E36" s="13">
-        <v>50</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>439</v>
-      </c>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>435</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="E37" s="14">
-        <v>190</v>
+        <v>0</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>439</v>
+        <v>89</v>
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="I37" s="13" t="s">
         <v>42</v>
@@ -3132,17 +3148,17 @@
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="E38" s="14">
-        <v>700</v>
+        <v>431</v>
+      </c>
+      <c r="E38" s="13">
+        <v>50</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>89</v>
+        <v>439</v>
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="13" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="I38" s="13" t="s">
         <v>42</v>
@@ -3165,17 +3181,17 @@
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="E39" s="14">
-        <v>5</v>
+        <v>190</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>89</v>
+        <v>439</v>
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="13" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="I39" s="13" t="s">
         <v>42</v>
@@ -3198,30 +3214,28 @@
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="13" t="s">
-        <v>448</v>
+        <v>432</v>
       </c>
       <c r="E40" s="14">
-        <v>14300</v>
+        <v>700</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="G40" s="13"/>
       <c r="H40" s="13" t="s">
-        <v>457</v>
+        <v>440</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>458</v>
+        <v>42</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>161</v>
+        <v>435</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="L40" s="13">
-        <v>32404477</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="L40" s="13"/>
       <c r="M40" s="13"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -3233,20 +3247,20 @@
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="13" t="s">
-        <v>461</v>
+        <v>433</v>
       </c>
       <c r="E41" s="14">
-        <v>941000</v>
+        <v>5</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>145</v>
+        <v>89</v>
       </c>
       <c r="G41" s="13"/>
       <c r="H41" s="13" t="s">
-        <v>463</v>
+        <v>441</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>462</v>
+        <v>42</v>
       </c>
       <c r="J41" s="13" t="s">
         <v>435</v>
@@ -3254,74 +3268,142 @@
       <c r="K41" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="L41" s="13">
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="13">
+        <v>1</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="E42" s="14">
+        <v>14300</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L42" s="13">
+        <v>32404477</v>
+      </c>
+      <c r="M42" s="13"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="13">
+        <v>1</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="E43" s="14">
+        <v>941000</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="K43" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L43" s="13">
         <v>15358653</v>
       </c>
-      <c r="M41" s="13"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A42" s="12">
-        <v>1</v>
-      </c>
-      <c r="B42" s="12" t="s">
+      <c r="M43" s="13"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="12">
+        <v>1</v>
+      </c>
+      <c r="B44" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12" t="s">
+      <c r="C44" s="12"/>
+      <c r="D44" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E44" s="12">
         <v>1.33E-12</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F44" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12" t="s">
+      <c r="G44" s="12"/>
+      <c r="H44" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I42" s="12" t="s">
+      <c r="I44" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12" t="s">
+      <c r="J44" s="12"/>
+      <c r="K44" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="L42" s="12">
+      <c r="L44" s="12">
         <v>7103258</v>
       </c>
-      <c r="M42" s="12" t="s">
+      <c r="M44" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="N42" s="12"/>
-      <c r="O42" s="12"/>
-      <c r="P42" s="12"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A43" s="12">
-        <v>1</v>
-      </c>
-      <c r="B43" s="12" t="s">
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="12">
+        <v>1</v>
+      </c>
+      <c r="B45" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12" t="s">
+      <c r="C45" s="12"/>
+      <c r="D45" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="E43" s="16">
+      <c r="E45" s="16">
         <v>1000</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F45" s="12" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H65">
+    <row r="67" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H67">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H4:M42" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="H4:M44" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3329,13 +3411,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G41" sqref="G41"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3471,25 +3553,29 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="11">
+        <v>0</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J7" s="11"/>
+      <c r="K7" s="11" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3501,120 +3587,124 @@
         <v>245</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>282</v>
+        <v>481</v>
       </c>
       <c r="G8" t="s">
         <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K8" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
-        <v>1</v>
-      </c>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="11">
+        <v>0</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" t="s">
+        <v>482</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" t="s">
+        <v>283</v>
+      </c>
+      <c r="K10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13" t="s">
         <v>444</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13" t="s">
+      <c r="E11" s="13"/>
+      <c r="F11" s="13" t="s">
         <v>445</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13" t="s">
         <v>446</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13" t="s">
+      <c r="J11" s="13"/>
+      <c r="K11" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
-        <v>1</v>
-      </c>
-      <c r="B10" s="13" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>1</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13" t="s">
+      <c r="E12" s="13"/>
+      <c r="F12" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G12" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13" t="s">
+      <c r="H12" s="13"/>
+      <c r="I12" s="13" t="s">
         <v>443</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>447</v>
       </c>
-      <c r="K10" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>245</v>
-      </c>
-      <c r="D11" t="s">
-        <v>254</v>
-      </c>
-      <c r="F11" t="s">
-        <v>255</v>
-      </c>
-      <c r="G11" t="s">
-        <v>256</v>
-      </c>
-      <c r="I11" t="s">
-        <v>257</v>
-      </c>
-      <c r="K11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>245</v>
-      </c>
-      <c r="D12" t="s">
-        <v>258</v>
-      </c>
-      <c r="F12" t="s">
-        <v>259</v>
-      </c>
-      <c r="G12" t="s">
-        <v>256</v>
-      </c>
-      <c r="I12" t="s">
-        <v>260</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="K12" s="13" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3626,19 +3716,19 @@
         <v>245</v>
       </c>
       <c r="D13" t="s">
-        <v>317</v>
+        <v>254</v>
       </c>
       <c r="F13" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="G13" t="s">
         <v>256</v>
       </c>
       <c r="I13" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="K13" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -3649,19 +3739,19 @@
         <v>245</v>
       </c>
       <c r="D14" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="F14" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="G14" t="s">
         <v>256</v>
       </c>
       <c r="I14" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="K14" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3672,16 +3762,16 @@
         <v>245</v>
       </c>
       <c r="D15" t="s">
-        <v>267</v>
+        <v>317</v>
       </c>
       <c r="F15" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="G15" t="s">
         <v>256</v>
       </c>
       <c r="I15" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="K15" t="s">
         <v>144</v>
@@ -3695,19 +3785,19 @@
         <v>245</v>
       </c>
       <c r="D16" t="s">
-        <v>356</v>
+        <v>263</v>
       </c>
       <c r="F16" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G16" t="s">
         <v>256</v>
       </c>
       <c r="I16" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="K16" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -3718,19 +3808,19 @@
         <v>245</v>
       </c>
       <c r="D17" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F17" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="G17" t="s">
         <v>256</v>
       </c>
       <c r="I17" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="K17" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -3741,45 +3831,41 @@
         <v>245</v>
       </c>
       <c r="D18" t="s">
-        <v>270</v>
+        <v>356</v>
       </c>
       <c r="F18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G18" t="s">
         <v>256</v>
       </c>
       <c r="I18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K18" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="13">
-        <v>1</v>
-      </c>
-      <c r="B19" s="13" t="s">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
         <v>245</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13" t="s">
-        <v>424</v>
-      </c>
-      <c r="G19" s="13" t="s">
+      <c r="D19" t="s">
+        <v>269</v>
+      </c>
+      <c r="F19" t="s">
+        <v>272</v>
+      </c>
+      <c r="G19" t="s">
         <v>256</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13" t="s">
+      <c r="I19" t="s">
+        <v>275</v>
+      </c>
+      <c r="K19" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3791,45 +3877,45 @@
         <v>245</v>
       </c>
       <c r="D20" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F20" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G20" t="s">
         <v>256</v>
       </c>
       <c r="I20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="K20" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
-        <v>0</v>
-      </c>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="13">
+        <v>1</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11" t="s">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3841,42 +3927,46 @@
         <v>245</v>
       </c>
       <c r="D22" t="s">
-        <v>465</v>
+        <v>277</v>
       </c>
       <c r="F22" t="s">
-        <v>474</v>
+        <v>278</v>
       </c>
       <c r="G22" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="I22" t="s">
-        <v>464</v>
+        <v>279</v>
       </c>
       <c r="K22" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="A23" s="11">
+        <v>0</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="D23" t="s">
-        <v>326</v>
-      </c>
-      <c r="F23" t="s">
-        <v>325</v>
-      </c>
-      <c r="G23" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" t="s">
-        <v>327</v>
-      </c>
-      <c r="K23" t="s">
-        <v>65</v>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -3887,19 +3977,19 @@
         <v>245</v>
       </c>
       <c r="D24" t="s">
-        <v>328</v>
+        <v>465</v>
       </c>
       <c r="F24" t="s">
-        <v>329</v>
+        <v>474</v>
       </c>
       <c r="G24" t="s">
-        <v>89</v>
+        <v>247</v>
       </c>
       <c r="I24" t="s">
-        <v>330</v>
+        <v>464</v>
       </c>
       <c r="K24" t="s">
-        <v>65</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -3910,16 +4000,16 @@
         <v>245</v>
       </c>
       <c r="D25" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="F25" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="G25" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="I25" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="K25" t="s">
         <v>65</v>
@@ -3933,16 +4023,16 @@
         <v>245</v>
       </c>
       <c r="D26" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F26" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="G26" t="s">
         <v>89</v>
       </c>
       <c r="I26" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="K26" t="s">
         <v>65</v>
@@ -3956,19 +4046,19 @@
         <v>245</v>
       </c>
       <c r="D27" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="F27" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="G27" t="s">
-        <v>256</v>
+        <v>89</v>
       </c>
       <c r="I27" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="K27" t="s">
-        <v>340</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -3979,19 +4069,19 @@
         <v>245</v>
       </c>
       <c r="D28" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="F28" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G28" t="s">
-        <v>256</v>
+        <v>89</v>
       </c>
       <c r="I28" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="K28" t="s">
-        <v>340</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -4002,16 +4092,16 @@
         <v>245</v>
       </c>
       <c r="D29" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="F29" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="G29" t="s">
         <v>256</v>
       </c>
       <c r="I29" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="K29" t="s">
         <v>340</v>
@@ -4025,19 +4115,19 @@
         <v>245</v>
       </c>
       <c r="D30" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="F30" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="G30" t="s">
         <v>256</v>
       </c>
       <c r="I30" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="K30" t="s">
-        <v>75</v>
+        <v>340</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -4048,19 +4138,19 @@
         <v>245</v>
       </c>
       <c r="D31" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="F31" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="G31" t="s">
         <v>256</v>
       </c>
       <c r="I31" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="K31" t="s">
-        <v>75</v>
+        <v>340</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -4071,16 +4161,16 @@
         <v>245</v>
       </c>
       <c r="D32" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="F32" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="G32" t="s">
         <v>256</v>
       </c>
       <c r="I32" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="K32" t="s">
         <v>75</v>
@@ -4094,19 +4184,19 @@
         <v>245</v>
       </c>
       <c r="D33" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="F33" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="G33" t="s">
-        <v>89</v>
+        <v>256</v>
       </c>
       <c r="I33" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="K33" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -4117,19 +4207,19 @@
         <v>245</v>
       </c>
       <c r="D34" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="F34" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="G34" t="s">
-        <v>89</v>
+        <v>256</v>
       </c>
       <c r="I34" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="K34" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -4140,10 +4230,10 @@
         <v>245</v>
       </c>
       <c r="D35" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F35" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="G35" t="s">
         <v>89</v>
@@ -4152,34 +4242,30 @@
         <v>359</v>
       </c>
       <c r="K35" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="11">
-        <v>0</v>
-      </c>
-      <c r="B36" s="11" t="s">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
         <v>245</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="G36" s="11" t="s">
+      <c r="D36" t="s">
+        <v>360</v>
+      </c>
+      <c r="F36" t="s">
+        <v>361</v>
+      </c>
+      <c r="G36" t="s">
         <v>89</v>
       </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11" t="s">
-        <v>398</v>
-      </c>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11" t="s">
-        <v>161</v>
+      <c r="I36" t="s">
+        <v>359</v>
+      </c>
+      <c r="K36" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -4190,98 +4276,148 @@
         <v>245</v>
       </c>
       <c r="D37" t="s">
-        <v>397</v>
+        <v>362</v>
       </c>
       <c r="F37" t="s">
-        <v>421</v>
+        <v>363</v>
       </c>
       <c r="G37" t="s">
         <v>89</v>
       </c>
       <c r="I37" t="s">
-        <v>398</v>
+        <v>359</v>
       </c>
       <c r="K37" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="13">
-        <v>1</v>
-      </c>
-      <c r="B38" s="13" t="s">
+      <c r="A38" s="11">
+        <v>0</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13" t="s">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>245</v>
+      </c>
+      <c r="D39" t="s">
+        <v>397</v>
+      </c>
+      <c r="F39" t="s">
+        <v>421</v>
+      </c>
+      <c r="G39" t="s">
+        <v>89</v>
+      </c>
+      <c r="I39" t="s">
+        <v>398</v>
+      </c>
+      <c r="K39" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="13">
+        <v>1</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13" t="s">
+      <c r="E40" s="13"/>
+      <c r="F40" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="G38" s="13" t="s">
+      <c r="G40" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13" t="s">
+      <c r="H40" s="13"/>
+      <c r="I40" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13" t="s">
+      <c r="J40" s="13"/>
+      <c r="K40" s="13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="13">
-        <v>1</v>
-      </c>
-      <c r="B39" s="13" t="s">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="13">
+        <v>1</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13" t="s">
+      <c r="C41" s="13"/>
+      <c r="D41" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13" t="s">
+      <c r="E41" s="13"/>
+      <c r="F41" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="G41" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13" t="s">
+      <c r="H41" s="13"/>
+      <c r="I41" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13" t="s">
+      <c r="J41" s="13"/>
+      <c r="K41" s="13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
         <v>245</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D42" t="s">
         <v>430</v>
       </c>
-      <c r="E40">
+      <c r="E42">
         <v>0</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G42" t="s">
         <v>89</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I42" t="s">
         <v>434</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J42" t="s">
         <v>42</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K42" t="s">
         <v>435</v>
       </c>
     </row>
@@ -5094,7 +5230,7 @@
         <v>75</v>
       </c>
       <c r="E19" s="5">
-        <v>2E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="G19" t="s">
         <v>145</v>
@@ -5219,13 +5355,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5340,28 +5476,31 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="11">
+        <v>0</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J6" s="11"/>
+      <c r="K6" s="11" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5373,47 +5512,50 @@
         <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>318</v>
+        <v>479</v>
       </c>
       <c r="F7" t="s">
         <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="11">
+        <v>0</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" t="s">
-        <v>59</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="G8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5425,19 +5567,19 @@
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>480</v>
       </c>
       <c r="F9" t="s">
         <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K9" t="s">
         <v>65</v>
@@ -5451,19 +5593,19 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
         <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K10" t="s">
         <v>65</v>
@@ -5477,22 +5619,22 @@
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="K11" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -5503,22 +5645,22 @@
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>237</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>236</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="I12" t="s">
-        <v>241</v>
+        <v>61</v>
       </c>
       <c r="K12" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -5529,19 +5671,19 @@
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>364</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
         <v>92</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K13" t="s">
         <v>116</v>
@@ -5555,10 +5697,10 @@
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>237</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>236</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -5567,38 +5709,35 @@
         <v>94</v>
       </c>
       <c r="I14" t="s">
-        <v>105</v>
+        <v>241</v>
       </c>
       <c r="K14" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
-        <v>0</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="F15" s="11" t="s">
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" t="s">
+        <v>364</v>
+      </c>
+      <c r="F15" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11" t="s">
+      <c r="G15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" t="s">
         <v>116</v>
       </c>
     </row>
@@ -5610,47 +5749,50 @@
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E16" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="F16" t="s">
         <v>92</v>
       </c>
       <c r="G16" t="s">
-        <v>415</v>
+        <v>94</v>
       </c>
       <c r="I16" t="s">
-        <v>416</v>
+        <v>105</v>
       </c>
       <c r="K16" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="A17" s="11">
+        <v>0</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" t="s">
-        <v>107</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G17" t="s">
-        <v>108</v>
-      </c>
-      <c r="I17" t="s">
-        <v>109</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="G17" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11" t="s">
         <v>116</v>
       </c>
     </row>
@@ -5662,19 +5804,19 @@
         <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E18" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F18" t="s">
         <v>92</v>
       </c>
       <c r="G18" t="s">
-        <v>112</v>
+        <v>415</v>
       </c>
       <c r="I18" t="s">
-        <v>113</v>
+        <v>416</v>
       </c>
       <c r="K18" t="s">
         <v>116</v>
@@ -5688,22 +5830,22 @@
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E19" t="s">
-        <v>164</v>
+        <v>107</v>
       </c>
       <c r="F19" t="s">
         <v>92</v>
       </c>
       <c r="G19" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="I19" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="K19" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -5714,22 +5856,22 @@
         <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>238</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>239</v>
+        <v>111</v>
       </c>
       <c r="F20" t="s">
         <v>92</v>
       </c>
       <c r="G20" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="I20" t="s">
-        <v>240</v>
+        <v>113</v>
       </c>
       <c r="K20" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -5740,19 +5882,19 @@
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>365</v>
+        <v>164</v>
       </c>
       <c r="F21" t="s">
         <v>92</v>
       </c>
       <c r="G21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K21" t="s">
         <v>144</v>
@@ -5766,10 +5908,10 @@
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>119</v>
+        <v>238</v>
       </c>
       <c r="E22" t="s">
-        <v>132</v>
+        <v>239</v>
       </c>
       <c r="F22" t="s">
         <v>92</v>
@@ -5778,38 +5920,35 @@
         <v>128</v>
       </c>
       <c r="I22" t="s">
-        <v>148</v>
+        <v>240</v>
       </c>
       <c r="K22" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="11">
-        <v>0</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F23" s="11" t="s">
+      <c r="D23" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" t="s">
+        <v>365</v>
+      </c>
+      <c r="F23" t="s">
         <v>92</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11" t="s">
-        <v>387</v>
-      </c>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11" t="s">
+      <c r="G23" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" t="s">
+        <v>147</v>
+      </c>
+      <c r="K23" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5821,47 +5960,50 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F24" t="s">
         <v>92</v>
       </c>
       <c r="G24" t="s">
-        <v>417</v>
+        <v>128</v>
       </c>
       <c r="I24" t="s">
-        <v>418</v>
+        <v>148</v>
       </c>
       <c r="K24" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="A25" s="11">
+        <v>0</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D25" t="s">
-        <v>135</v>
-      </c>
-      <c r="E25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G25" t="s">
-        <v>369</v>
-      </c>
-      <c r="I25" t="s">
-        <v>388</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="G25" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5873,108 +6015,102 @@
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="E26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F26" t="s">
         <v>92</v>
       </c>
       <c r="G26" t="s">
-        <v>139</v>
+        <v>417</v>
       </c>
       <c r="I26" t="s">
-        <v>138</v>
+        <v>418</v>
       </c>
       <c r="K26" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" t="s">
+        <v>136</v>
+      </c>
+      <c r="F27" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" t="s">
+        <v>369</v>
+      </c>
+      <c r="I27" t="s">
+        <v>388</v>
+      </c>
+      <c r="K27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" t="s">
+        <v>92</v>
+      </c>
+      <c r="G28" t="s">
+        <v>139</v>
+      </c>
+      <c r="I28" t="s">
+        <v>138</v>
+      </c>
+      <c r="K28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="11">
         <v>0</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E29" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G29" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11" t="s">
+      <c r="H29" s="11"/>
+      <c r="I29" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="12">
-        <v>1</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="12">
-        <v>1</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12" t="s">
+      <c r="J29" s="11"/>
+      <c r="K29" s="11" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5987,20 +6123,20 @@
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12" t="s">
-        <v>143</v>
+        <v>297</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12" t="s">
@@ -6016,24 +6152,24 @@
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>83</v>
+        <v>298</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>302</v>
+        <v>131</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -6045,24 +6181,24 @@
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12" t="s">
-        <v>300</v>
+        <v>140</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>304</v>
+        <v>141</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>305</v>
+        <v>142</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>306</v>
+        <v>143</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -6074,20 +6210,20 @@
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>366</v>
+        <v>83</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="12" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="12" t="s">
@@ -6103,10 +6239,10 @@
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
-        <v>123</v>
+        <v>300</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>413</v>
+        <v>304</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>92</v>
@@ -6116,7 +6252,7 @@
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="12" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12" t="s">
@@ -6124,31 +6260,31 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="11">
-        <v>0</v>
-      </c>
-      <c r="B35" s="11" t="s">
+      <c r="A35" s="12">
+        <v>1</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="F35" s="11" t="s">
+      <c r="C35" s="12"/>
+      <c r="D35" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="F35" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G35" s="11" t="s">
-        <v>370</v>
-      </c>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11" t="s">
-        <v>389</v>
-      </c>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11" t="s">
+      <c r="G35" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12" t="s">
         <v>161</v>
       </c>
     </row>
@@ -6161,20 +6297,20 @@
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>419</v>
+        <v>305</v>
       </c>
       <c r="H36" s="12"/>
       <c r="I36" s="12" t="s">
-        <v>420</v>
+        <v>309</v>
       </c>
       <c r="J36" s="12"/>
       <c r="K36" s="12" t="s">
@@ -6182,31 +6318,31 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="12">
-        <v>1</v>
-      </c>
-      <c r="B37" s="12" t="s">
+      <c r="A37" s="11">
+        <v>0</v>
+      </c>
+      <c r="B37" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="F37" s="12" t="s">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="F37" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G37" s="12" t="s">
-        <v>311</v>
-      </c>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12" t="s">
+      <c r="G37" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11" t="s">
         <v>161</v>
       </c>
     </row>
@@ -6219,20 +6355,20 @@
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="12" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>151</v>
+        <v>414</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>92</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>152</v>
+        <v>419</v>
       </c>
       <c r="H38" s="12"/>
       <c r="I38" s="12" t="s">
-        <v>153</v>
+        <v>420</v>
       </c>
       <c r="J38" s="12"/>
       <c r="K38" s="12" t="s">
@@ -6240,57 +6376,60 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="A39" s="12">
+        <v>1</v>
+      </c>
+      <c r="B39" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D39" t="s">
-        <v>154</v>
-      </c>
-      <c r="E39" t="s">
-        <v>228</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="C39" s="12"/>
+      <c r="D39" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="F39" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G39" t="s">
-        <v>155</v>
-      </c>
-      <c r="I39" t="s">
-        <v>156</v>
-      </c>
-      <c r="K39" t="s">
+      <c r="G39" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="11">
-        <v>0</v>
-      </c>
-      <c r="B40" s="11" t="s">
+      <c r="A40" s="12">
+        <v>1</v>
+      </c>
+      <c r="B40" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="F40" s="11" t="s">
+      <c r="C40" s="12"/>
+      <c r="D40" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G40" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11" t="s">
+      <c r="G40" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12" t="s">
         <v>161</v>
       </c>
     </row>
@@ -6302,19 +6441,19 @@
         <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>208</v>
+        <v>154</v>
       </c>
       <c r="E41" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="F41" t="s">
         <v>92</v>
       </c>
       <c r="G41" t="s">
-        <v>403</v>
+        <v>155</v>
       </c>
       <c r="I41" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
       <c r="K41" t="s">
         <v>161</v>
@@ -6329,20 +6468,20 @@
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F42" s="11" t="s">
         <v>92</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="H42" s="11"/>
       <c r="I42" s="11" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="J42" s="11"/>
       <c r="K42" s="11" t="s">
@@ -6357,157 +6496,160 @@
         <v>35</v>
       </c>
       <c r="D43" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="E43" t="s">
-        <v>410</v>
+        <v>209</v>
       </c>
       <c r="F43" t="s">
         <v>92</v>
       </c>
       <c r="G43" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I43" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="K43" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="A44" s="11">
+        <v>0</v>
+      </c>
+      <c r="B44" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D44" t="s">
+      <c r="C44" s="11"/>
+      <c r="D44" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45" t="s">
+        <v>410</v>
+      </c>
+      <c r="F45" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" t="s">
+        <v>404</v>
+      </c>
+      <c r="I45" t="s">
+        <v>202</v>
+      </c>
+      <c r="K45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" t="s">
         <v>158</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E46" t="s">
         <v>162</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F46" t="s">
         <v>92</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G46" t="s">
         <v>371</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I46" t="s">
         <v>390</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K46" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="13">
-        <v>1</v>
-      </c>
-      <c r="B45" s="13" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="13">
+        <v>1</v>
+      </c>
+      <c r="B47" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13" t="s">
+      <c r="C47" s="13"/>
+      <c r="D47" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E47" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="F47" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G45" s="13" t="s">
+      <c r="G47" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13" t="s">
+      <c r="H47" s="13"/>
+      <c r="I47" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13" t="s">
+      <c r="J47" s="13"/>
+      <c r="K47" s="13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="11">
         <v>0</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B48" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11" t="s">
+      <c r="C48" s="11"/>
+      <c r="D48" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F48" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G46" s="11" t="s">
+      <c r="G48" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11" t="s">
+      <c r="H48" s="11"/>
+      <c r="I48" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" t="s">
-        <v>159</v>
-      </c>
-      <c r="E47" t="s">
-        <v>163</v>
-      </c>
-      <c r="F47" t="s">
-        <v>92</v>
-      </c>
-      <c r="G47" t="s">
-        <v>381</v>
-      </c>
-      <c r="I47" t="s">
-        <v>382</v>
-      </c>
-      <c r="K47" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E48" t="s">
-        <v>82</v>
-      </c>
-      <c r="F48" t="s">
-        <v>92</v>
-      </c>
-      <c r="G48" t="s">
-        <v>165</v>
-      </c>
-      <c r="I48" t="s">
-        <v>166</v>
-      </c>
-      <c r="K48" t="s">
+      <c r="J48" s="11"/>
+      <c r="K48" s="11" t="s">
         <v>161</v>
       </c>
     </row>
@@ -6519,26 +6661,78 @@
         <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>383</v>
+        <v>159</v>
       </c>
       <c r="E49" t="s">
-        <v>393</v>
+        <v>163</v>
       </c>
       <c r="F49" t="s">
         <v>92</v>
       </c>
       <c r="G49" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I49" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="K49" t="s">
         <v>161</v>
       </c>
     </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" t="s">
+        <v>92</v>
+      </c>
+      <c r="G50" t="s">
+        <v>165</v>
+      </c>
+      <c r="I50" t="s">
+        <v>166</v>
+      </c>
+      <c r="K50" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" t="s">
+        <v>383</v>
+      </c>
+      <c r="E51" t="s">
+        <v>393</v>
+      </c>
+      <c r="F51" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" t="s">
+        <v>384</v>
+      </c>
+      <c r="I51" t="s">
+        <v>385</v>
+      </c>
+      <c r="K51" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A4:K49" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A4:K51" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>